<commit_message>
flangesegments validation: added fatigue damage to validation sheets
</commit_message>
<xml_diff>
--- a/validations/flangesegments.PolynomialLFlangeSegment/Case_1_D7500_L_Tilt-0p00deg_ShapeFactor-1p00_Fv2800kN_ShellStiff-Interp.xlsx
+++ b/validations/flangesegments.PolynomialLFlangeSegment/Case_1_D7500_L_Tilt-0p00deg_ShapeFactor-1p00_Fv2800kN_ShellStiff-Interp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MarcelloB\mdb\!Progetti\!KCI\!SP2200052 - Bolt &amp; Beautiful\!pyflange-package\validations\flangesegments.PolynomialLFlangeSegment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FCC11F5-FC62-4690-B420-2F7B1FB48671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{598D23D1-7330-4882-9AD8-D4D55505B091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-8700" windowWidth="29040" windowHeight="18240" xr2:uid="{710C990D-69B5-462C-923E-A1886280CCCB}"/>
   </bookViews>
@@ -37,6 +37,7 @@
     <definedName name="b" localSheetId="1">PyFlange_Gap30deg!$J$37</definedName>
     <definedName name="b" localSheetId="2">PyFlange_Gap60deg!$J$37</definedName>
     <definedName name="b" localSheetId="3">PyFlange_Gap90deg!$J$37</definedName>
+    <definedName name="bending_factor" localSheetId="5">SGRE!$P$16</definedName>
     <definedName name="bolt.As" localSheetId="4">PyFlange_Gap120deg!$J$157</definedName>
     <definedName name="bolt.As" localSheetId="1">PyFlange_Gap30deg!$J$157</definedName>
     <definedName name="bolt.As" localSheetId="2">PyFlange_Gap60deg!$J$157</definedName>
@@ -158,6 +159,12 @@
     <definedName name="E_mod" localSheetId="1">PyFlange_Gap30deg!$J$43</definedName>
     <definedName name="E_mod" localSheetId="2">PyFlange_Gap60deg!$J$43</definedName>
     <definedName name="E_mod" localSheetId="3">PyFlange_Gap90deg!$J$43</definedName>
+    <definedName name="fatigue.damage" localSheetId="4">PyFlange_Gap120deg!$J$169</definedName>
+    <definedName name="fatigue.damage" localSheetId="1">PyFlange_Gap30deg!$J$169</definedName>
+    <definedName name="fatigue.damage" localSheetId="2">PyFlange_Gap60deg!$J$169</definedName>
+    <definedName name="fatigue.damage" localSheetId="3">PyFlange_Gap90deg!$J$169</definedName>
+    <definedName name="fatigue.size_exponent" localSheetId="5">SGRE!$P$7</definedName>
+    <definedName name="fatigue.size_factor" localSheetId="5">SGRE!$P$8</definedName>
     <definedName name="ffff" localSheetId="5">#REF!</definedName>
     <definedName name="ffff">#REF!</definedName>
     <definedName name="fffff" localSheetId="5">#REF!</definedName>
@@ -251,6 +258,10 @@
     <definedName name="k_seg" localSheetId="1">PyFlange_Gap30deg!$J$142</definedName>
     <definedName name="k_seg" localSheetId="2">PyFlange_Gap60deg!$J$142</definedName>
     <definedName name="k_seg" localSheetId="3">PyFlange_Gap90deg!$J$142</definedName>
+    <definedName name="markov_matrix" localSheetId="5">SGRE!$U$16:$W$1216</definedName>
+    <definedName name="markov_matrix.cycles" localSheetId="5">SGRE!$W$16:$W$1216</definedName>
+    <definedName name="markov_matrix.mean" localSheetId="5">SGRE!$V$16:$V$1216</definedName>
+    <definedName name="markov_matrix.range" localSheetId="5">SGRE!$U$16:$U$1216</definedName>
     <definedName name="Ms_coeff.comp.0" localSheetId="4">PyFlange_Gap120deg!$I$120</definedName>
     <definedName name="Ms_coeff.comp.0" localSheetId="1">PyFlange_Gap30deg!$I$120</definedName>
     <definedName name="Ms_coeff.comp.0" localSheetId="2">PyFlange_Gap60deg!$I$120</definedName>
@@ -331,15 +342,17 @@
     <definedName name="polynomial_initial_slope" localSheetId="1">PyFlange_Gap30deg!$J$152</definedName>
     <definedName name="polynomial_initial_slope" localSheetId="2">PyFlange_Gap60deg!$J$152</definedName>
     <definedName name="polynomial_initial_slope" localSheetId="3">PyFlange_Gap90deg!$J$152</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="4">PyFlange_Gap120deg!$A$11:$K$176</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">PyFlange_Gap30deg!$A$11:$K$176</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">PyFlange_Gap60deg!$A$11:$K$176</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">PyFlange_Gap90deg!$A$11:$K$176</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">PyFlange_Gap120deg!$A$11:$K$178</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">PyFlange_Gap30deg!$A$11:$K$178</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">PyFlange_Gap60deg!$A$11:$K$178</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">PyFlange_Gap90deg!$A$11:$K$178</definedName>
     <definedName name="query">#N/A</definedName>
     <definedName name="Radius" localSheetId="4">PyFlange_Gap120deg!$J$41</definedName>
     <definedName name="Radius" localSheetId="1">PyFlange_Gap30deg!$J$41</definedName>
     <definedName name="Radius" localSheetId="2">PyFlange_Gap60deg!$J$41</definedName>
     <definedName name="Radius" localSheetId="3">PyFlange_Gap90deg!$J$41</definedName>
+    <definedName name="SF_load" localSheetId="5">SGRE!$P$14</definedName>
+    <definedName name="SF_material" localSheetId="5">SGRE!$P$15</definedName>
     <definedName name="sheet_name" localSheetId="0">Comparison!$AA$2</definedName>
     <definedName name="shell_thickness" localSheetId="4">PyFlange_Gap120deg!$J$38</definedName>
     <definedName name="shell_thickness" localSheetId="1">PyFlange_Gap30deg!$J$38</definedName>
@@ -495,7 +508,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2001" uniqueCount="413">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2019" uniqueCount="416">
   <si>
     <t>A</t>
   </si>
@@ -4473,12 +4486,21 @@
   <si>
     <t>Design value capped to 90% Fp,C*: Yes</t>
   </si>
+  <si>
+    <t>Fatigue</t>
+  </si>
+  <si>
+    <t>Cumulated damage:</t>
+  </si>
+  <si>
+    <t>D =</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="11">
+  <numFmts count="12">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
@@ -4490,6 +4512,7 @@
     <numFmt numFmtId="172" formatCode="0.000000"/>
     <numFmt numFmtId="173" formatCode="0.00000000000000000000"/>
     <numFmt numFmtId="174" formatCode="0.000000000"/>
+    <numFmt numFmtId="175" formatCode="0.00000"/>
   </numFmts>
   <fonts count="68">
     <font>
@@ -5369,7 +5392,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="190">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -5863,13 +5886,34 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="13" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="2" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="5" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5881,61 +5925,11 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="21" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="2" borderId="20" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="13" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="47" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="171" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="11" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="9">
@@ -5949,7 +5943,14 @@
     <cellStyle name="Standard 2 4" xfId="7" xr:uid="{FDF43DE4-8234-4C19-B917-E06AD07C46BA}"/>
     <cellStyle name="Standard 2 5" xfId="8" xr:uid="{321FB54D-E4D1-4E0E-94BC-7ABFCC6C7A69}"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="29">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FFFF0000"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF00B050"/>
@@ -20570,8 +20571,8 @@
   <dimension ref="A1:AA114"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H49" sqref="H49"/>
+      <pane ySplit="4" topLeftCell="A92" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -20602,7 +20603,7 @@
       <c r="F2" s="155"/>
       <c r="G2" s="163">
         <f ca="1">MAX(MAX(G5:G114),ABS(MIN(G5:G114)))</f>
-        <v>3.0843681232673666E-2</v>
+        <v>4.0998890756861528E-2</v>
       </c>
       <c r="V2" s="158">
         <v>30</v>
@@ -23003,11 +23004,13 @@
         <f t="array" ref="E114">INDEX(SGRE!L136:O136,case_number)</f>
         <v>1.4812583073587486</v>
       </c>
-      <c r="F114" s="109" t="s">
-        <v>85</v>
-      </c>
-      <c r="G114" s="109" t="s">
-        <v>85</v>
+      <c r="F114" s="109" cm="1">
+        <f t="array" aca="1" ref="F114" ca="1">INDIRECT(sheet_name&amp;"!fatigue.damage")</f>
+        <v>1.4205283598326537</v>
+      </c>
+      <c r="G114" s="118">
+        <f ca="1">(F114-E114)/E114</f>
+        <v>-4.0998890756861528E-2</v>
       </c>
       <c r="H114" t="s">
         <v>341</v>
@@ -23015,97 +23018,103 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2 G76:G80">
-    <cfRule type="cellIs" dxfId="27" priority="1" operator="notBetween">
+    <cfRule type="cellIs" dxfId="28" priority="2" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7:G9">
+    <cfRule type="cellIs" dxfId="27" priority="20" operator="notBetween">
+      <formula>-0.001</formula>
+      <formula>0.001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G14:G16">
     <cfRule type="cellIs" dxfId="26" priority="19" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G14:G16">
+  <conditionalFormatting sqref="G26:G31">
     <cfRule type="cellIs" dxfId="25" priority="18" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G26:G31">
+  <conditionalFormatting sqref="G38:G39">
     <cfRule type="cellIs" dxfId="24" priority="17" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38:G39">
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="notBetween">
+  <conditionalFormatting sqref="G45:G50">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G45:G50">
+  <conditionalFormatting sqref="G54:G57">
     <cfRule type="cellIs" dxfId="22" priority="5" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G54:G57">
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="notBetween">
+  <conditionalFormatting sqref="G59:G63">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G59:G63">
+  <conditionalFormatting sqref="G65:G68">
     <cfRule type="cellIs" dxfId="20" priority="14" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G65:G68">
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="notBetween">
-      <formula>-0.001</formula>
-      <formula>0.001</formula>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="G71">
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="notBetween">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G73:G74">
-    <cfRule type="cellIs" dxfId="17" priority="12" operator="notBetween">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G83">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="notBetween">
+      <formula>-0.001</formula>
+      <formula>0.001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G85:G87">
     <cfRule type="cellIs" dxfId="16" priority="10" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G85:G87">
+  <conditionalFormatting sqref="G91:G92">
     <cfRule type="cellIs" dxfId="15" priority="9" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G91:G92">
+  <conditionalFormatting sqref="G96">
     <cfRule type="cellIs" dxfId="14" priority="8" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G96">
+  <conditionalFormatting sqref="G98">
     <cfRule type="cellIs" dxfId="13" priority="7" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G98">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="notBetween">
+  <conditionalFormatting sqref="G114">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="notBetween">
       <formula>-0.001</formula>
       <formula>0.001</formula>
     </cfRule>
@@ -23126,11 +23135,11 @@
     <tabColor theme="0" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DJ180"/>
+  <dimension ref="A1:DJ182"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="Q13" sqref="Q13"/>
+      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="R167" sqref="R167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -23216,12 +23225,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
-      <c r="F5" s="185"/>
-      <c r="G5" s="186"/>
+      <c r="B5" s="175"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="177"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -23229,12 +23238,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="186"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="177"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -23242,12 +23251,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="184"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="185"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="185"/>
-      <c r="G7" s="186"/>
+      <c r="B7" s="175"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -23255,12 +23264,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="184"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="185"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="185"/>
-      <c r="G8" s="186"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="177"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -23268,12 +23277,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="184"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="186"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="177"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -23321,112 +23330,112 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="178" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="176" t="s">
+      <c r="C13" s="178"/>
+      <c r="D13" s="180" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="176"/>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="177"/>
-      <c r="D14" s="176" t="s">
+      <c r="C14" s="178"/>
+      <c r="D14" s="180" t="s">
         <v>103</v>
       </c>
-      <c r="E14" s="176"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="176"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="176"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+      <c r="J14" s="180"/>
+      <c r="K14" s="180"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="176" t="s">
+      <c r="C15" s="178"/>
+      <c r="D15" s="180" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="176"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="176"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
+      <c r="J15" s="180"/>
+      <c r="K15" s="180"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="178" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="177"/>
-      <c r="D16" s="176" t="str">
+      <c r="C16" s="178"/>
+      <c r="D16" s="180" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 30° gap size</v>
       </c>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="180"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="177" t="s">
+      <c r="B17" s="178" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="177"/>
-      <c r="D17" s="175" t="s">
+      <c r="C17" s="178"/>
+      <c r="D17" s="184" t="s">
         <v>324</v>
       </c>
-      <c r="E17" s="176"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="180"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="180"/>
+      <c r="J17" s="180"/>
+      <c r="K17" s="180"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="177" t="s">
+      <c r="B18" s="178" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="177"/>
-      <c r="D18" s="187">
+      <c r="C18" s="178"/>
+      <c r="D18" s="179">
         <v>45432</v>
       </c>
-      <c r="E18" s="187"/>
-      <c r="F18" s="187"/>
-      <c r="G18" s="187"/>
-      <c r="H18" s="187"/>
-      <c r="I18" s="187"/>
-      <c r="J18" s="187"/>
-      <c r="K18" s="187"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="179"/>
+      <c r="K18" s="179"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -23614,16 +23623,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="179"/>
-      <c r="D28" s="179"/>
-      <c r="E28" s="179"/>
-      <c r="F28" s="179"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="179"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="180"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="186"/>
+      <c r="I28" s="186"/>
+      <c r="J28" s="186"/>
+      <c r="K28" s="187"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -27444,31 +27453,46 @@
       <c r="L167" s="3"/>
     </row>
     <row r="168" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A168" s="9"/>
-      <c r="B168" s="58"/>
-      <c r="C168" s="58"/>
-      <c r="D168" s="58"/>
-      <c r="E168" s="58"/>
-      <c r="F168" s="58"/>
-      <c r="G168" s="58"/>
-      <c r="H168" s="58"/>
-      <c r="I168" s="59"/>
-      <c r="J168" s="125"/>
-      <c r="K168" s="60"/>
+      <c r="A168" s="75" t="str">
+        <f>$A$124&amp;"."&amp;7</f>
+        <v>A.4.7</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
       <c r="L168" s="3"/>
     </row>
     <row r="169" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A169" s="9"/>
-      <c r="B169" s="58"/>
-      <c r="C169" s="58"/>
-      <c r="D169" s="58"/>
-      <c r="E169" s="58"/>
-      <c r="F169" s="58"/>
-      <c r="G169" s="58"/>
-      <c r="H169" s="58"/>
-      <c r="I169" s="59"/>
-      <c r="J169" s="125"/>
-      <c r="K169" s="60"/>
+      <c r="A169" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="11"/>
+      <c r="G169" s="11"/>
+      <c r="H169" s="11"/>
+      <c r="I169" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="J169" s="189">
+        <v>1.4205283598326537</v>
+      </c>
+      <c r="K169" s="93" t="s">
+        <v>85</v>
+      </c>
       <c r="L169" s="3"/>
     </row>
     <row r="170" spans="1:21" ht="20.100000000000001" customHeight="1">
@@ -27537,45 +27561,79 @@
       <c r="G174" s="58"/>
       <c r="H174" s="58"/>
       <c r="I174" s="59"/>
-      <c r="J174" s="63"/>
+      <c r="J174" s="125"/>
       <c r="K174" s="60"/>
       <c r="L174" s="3"/>
     </row>
     <row r="175" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A175" s="4"/>
-      <c r="B175" s="4"/>
-      <c r="C175" s="4"/>
-      <c r="D175" s="4"/>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
-      <c r="G175" s="4"/>
-      <c r="H175" s="4"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="58"/>
+      <c r="C175" s="58"/>
+      <c r="D175" s="58"/>
+      <c r="E175" s="58"/>
+      <c r="F175" s="58"/>
+      <c r="G175" s="58"/>
+      <c r="H175" s="58"/>
+      <c r="I175" s="59"/>
+      <c r="J175" s="125"/>
+      <c r="K175" s="60"/>
       <c r="L175" s="3"/>
     </row>
     <row r="176" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="4"/>
-      <c r="F176" s="4"/>
-      <c r="G176" s="4"/>
-      <c r="H176" s="4"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="4"/>
-      <c r="K176" s="4"/>
+      <c r="A176" s="9"/>
+      <c r="B176" s="58"/>
+      <c r="C176" s="58"/>
+      <c r="D176" s="58"/>
+      <c r="E176" s="58"/>
+      <c r="F176" s="58"/>
+      <c r="G176" s="58"/>
+      <c r="H176" s="58"/>
+      <c r="I176" s="59"/>
+      <c r="J176" s="63"/>
+      <c r="K176" s="60"/>
       <c r="L176" s="3"/>
     </row>
-    <row r="180" spans="2:4" ht="13.2">
-      <c r="B180" s="69"/>
-      <c r="C180" s="69"/>
-      <c r="D180" s="69"/>
+    <row r="177" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="3"/>
+    </row>
+    <row r="178" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="3"/>
+    </row>
+    <row r="182" spans="1:12" ht="13.2">
+      <c r="B182" s="69"/>
+      <c r="C182" s="69"/>
+      <c r="D182" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="B4:G4"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B7:G7"/>
     <mergeCell ref="B8:G8"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B18:C18"/>
@@ -27586,31 +27644,25 @@
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="D16:K16"/>
     <mergeCell ref="B17:C17"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B7:G7"/>
     <mergeCell ref="D17:K17"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B28:K28"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="11" priority="5" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="5" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="10" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="9" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -27633,11 +27685,11 @@
     <tabColor theme="0" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DJ180"/>
+  <dimension ref="A1:DJ182"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A147" sqref="A147:XFD147"/>
+      <pane ySplit="1" topLeftCell="A162" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J169" sqref="J169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -27723,12 +27775,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
-      <c r="F5" s="185"/>
-      <c r="G5" s="186"/>
+      <c r="B5" s="175"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="177"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -27736,12 +27788,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="186"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="177"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -27749,12 +27801,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="184"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="185"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="185"/>
-      <c r="G7" s="186"/>
+      <c r="B7" s="175"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -27762,12 +27814,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="184"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="185"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="185"/>
-      <c r="G8" s="186"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="177"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -27775,12 +27827,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="184"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="186"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="177"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -27828,117 +27880,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="178" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="176" t="str">
+      <c r="C13" s="178"/>
+      <c r="D13" s="180" t="str">
         <f>PyFlange_Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="176"/>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="177"/>
-      <c r="D14" s="176" t="str">
+      <c r="C14" s="178"/>
+      <c r="D14" s="180" t="str">
         <f>PyFlange_Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="176"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="176"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="176"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+      <c r="J14" s="180"/>
+      <c r="K14" s="180"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="176" t="str">
+      <c r="C15" s="178"/>
+      <c r="D15" s="180" t="str">
         <f>PyFlange_Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="176"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="176"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
+      <c r="J15" s="180"/>
+      <c r="K15" s="180"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="178" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="177"/>
-      <c r="D16" s="176" t="str">
+      <c r="C16" s="178"/>
+      <c r="D16" s="180" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 60° gap size</v>
       </c>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="180"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="177" t="s">
+      <c r="B17" s="178" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="177"/>
-      <c r="D17" s="176" t="str">
+      <c r="C17" s="178"/>
+      <c r="D17" s="180" t="str">
         <f>PyFlange_Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="176"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="180"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="180"/>
+      <c r="J17" s="180"/>
+      <c r="K17" s="180"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="177" t="s">
+      <c r="B18" s="178" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="177"/>
-      <c r="D18" s="187">
+      <c r="C18" s="178"/>
+      <c r="D18" s="179">
         <f>PyFlange_Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="187"/>
-      <c r="F18" s="187"/>
-      <c r="G18" s="187"/>
-      <c r="H18" s="187"/>
-      <c r="I18" s="187"/>
-      <c r="J18" s="187"/>
-      <c r="K18" s="187"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="179"/>
+      <c r="K18" s="179"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -28126,16 +28178,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="179"/>
-      <c r="D28" s="179"/>
-      <c r="E28" s="179"/>
-      <c r="F28" s="179"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="179"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="180"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="186"/>
+      <c r="I28" s="186"/>
+      <c r="J28" s="186"/>
+      <c r="K28" s="187"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -31929,31 +31981,46 @@
       <c r="L167" s="3"/>
     </row>
     <row r="168" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A168" s="9"/>
-      <c r="B168" s="58"/>
-      <c r="C168" s="58"/>
-      <c r="D168" s="58"/>
-      <c r="E168" s="58"/>
-      <c r="F168" s="58"/>
-      <c r="G168" s="58"/>
-      <c r="H168" s="58"/>
-      <c r="I168" s="59"/>
-      <c r="J168" s="125"/>
-      <c r="K168" s="60"/>
+      <c r="A168" s="75" t="str">
+        <f>$A$124&amp;"."&amp;7</f>
+        <v>B.4.7</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
       <c r="L168" s="3"/>
     </row>
     <row r="169" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A169" s="9"/>
-      <c r="B169" s="58"/>
-      <c r="C169" s="58"/>
-      <c r="D169" s="58"/>
-      <c r="E169" s="58"/>
-      <c r="F169" s="58"/>
-      <c r="G169" s="58"/>
-      <c r="H169" s="58"/>
-      <c r="I169" s="59"/>
-      <c r="J169" s="125"/>
-      <c r="K169" s="60"/>
+      <c r="A169" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="11"/>
+      <c r="G169" s="11"/>
+      <c r="H169" s="11"/>
+      <c r="I169" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="J169" s="189">
+        <v>3.2013675286014345</v>
+      </c>
+      <c r="K169" s="93" t="s">
+        <v>85</v>
+      </c>
       <c r="L169" s="3"/>
     </row>
     <row r="170" spans="1:21" ht="20.100000000000001" customHeight="1">
@@ -32022,45 +32089,80 @@
       <c r="G174" s="58"/>
       <c r="H174" s="58"/>
       <c r="I174" s="59"/>
-      <c r="J174" s="63"/>
+      <c r="J174" s="125"/>
       <c r="K174" s="60"/>
       <c r="L174" s="3"/>
     </row>
     <row r="175" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A175" s="4"/>
-      <c r="B175" s="4"/>
-      <c r="C175" s="4"/>
-      <c r="D175" s="4"/>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
-      <c r="G175" s="4"/>
-      <c r="H175" s="4"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="58"/>
+      <c r="C175" s="58"/>
+      <c r="D175" s="58"/>
+      <c r="E175" s="58"/>
+      <c r="F175" s="58"/>
+      <c r="G175" s="58"/>
+      <c r="H175" s="58"/>
+      <c r="I175" s="59"/>
+      <c r="J175" s="125"/>
+      <c r="K175" s="60"/>
       <c r="L175" s="3"/>
     </row>
     <row r="176" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="4"/>
-      <c r="F176" s="4"/>
-      <c r="G176" s="4"/>
-      <c r="H176" s="4"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="4"/>
-      <c r="K176" s="4"/>
+      <c r="A176" s="9"/>
+      <c r="B176" s="58"/>
+      <c r="C176" s="58"/>
+      <c r="D176" s="58"/>
+      <c r="E176" s="58"/>
+      <c r="F176" s="58"/>
+      <c r="G176" s="58"/>
+      <c r="H176" s="58"/>
+      <c r="I176" s="59"/>
+      <c r="J176" s="63"/>
+      <c r="K176" s="60"/>
       <c r="L176" s="3"/>
     </row>
-    <row r="180" spans="2:4" ht="13.2">
-      <c r="B180" s="69"/>
-      <c r="C180" s="69"/>
-      <c r="D180" s="69"/>
+    <row r="177" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="3"/>
+    </row>
+    <row r="178" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="3"/>
+    </row>
+    <row r="182" spans="1:12" ht="13.2">
+      <c r="B182" s="69"/>
+      <c r="C182" s="69"/>
+      <c r="D182" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -32074,28 +32176,21 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="8" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="3" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="7" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -32118,11 +32213,11 @@
     <tabColor theme="0" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DJ180"/>
+  <dimension ref="A1:DJ182"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A147" sqref="A147:XFD147"/>
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J169" sqref="J169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -32208,12 +32303,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
-      <c r="F5" s="185"/>
-      <c r="G5" s="186"/>
+      <c r="B5" s="175"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="177"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -32221,12 +32316,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="186"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="177"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -32234,12 +32329,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="184"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="185"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="185"/>
-      <c r="G7" s="186"/>
+      <c r="B7" s="175"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -32247,12 +32342,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="184"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="185"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="185"/>
-      <c r="G8" s="186"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="177"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -32260,12 +32355,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="184"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="186"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="177"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -32313,117 +32408,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="178" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="176" t="str">
+      <c r="C13" s="178"/>
+      <c r="D13" s="180" t="str">
         <f>PyFlange_Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="176"/>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="177"/>
-      <c r="D14" s="176" t="str">
+      <c r="C14" s="178"/>
+      <c r="D14" s="180" t="str">
         <f>PyFlange_Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="176"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="176"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="176"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+      <c r="J14" s="180"/>
+      <c r="K14" s="180"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="176" t="str">
+      <c r="C15" s="178"/>
+      <c r="D15" s="180" t="str">
         <f>PyFlange_Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="176"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="176"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
+      <c r="J15" s="180"/>
+      <c r="K15" s="180"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="178" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="177"/>
-      <c r="D16" s="176" t="str">
+      <c r="C16" s="178"/>
+      <c r="D16" s="180" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 90° gap size</v>
       </c>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="180"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="177" t="s">
+      <c r="B17" s="178" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="177"/>
-      <c r="D17" s="176" t="str">
+      <c r="C17" s="178"/>
+      <c r="D17" s="180" t="str">
         <f>PyFlange_Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="176"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="180"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="180"/>
+      <c r="J17" s="180"/>
+      <c r="K17" s="180"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="177" t="s">
+      <c r="B18" s="178" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="177"/>
-      <c r="D18" s="187">
+      <c r="C18" s="178"/>
+      <c r="D18" s="179">
         <f>PyFlange_Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="187"/>
-      <c r="F18" s="187"/>
-      <c r="G18" s="187"/>
-      <c r="H18" s="187"/>
-      <c r="I18" s="187"/>
-      <c r="J18" s="187"/>
-      <c r="K18" s="187"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="179"/>
+      <c r="K18" s="179"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -32611,16 +32706,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="179"/>
-      <c r="D28" s="179"/>
-      <c r="E28" s="179"/>
-      <c r="F28" s="179"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="179"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="180"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="186"/>
+      <c r="I28" s="186"/>
+      <c r="J28" s="186"/>
+      <c r="K28" s="187"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -36414,31 +36509,46 @@
       <c r="L167" s="3"/>
     </row>
     <row r="168" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A168" s="9"/>
-      <c r="B168" s="58"/>
-      <c r="C168" s="58"/>
-      <c r="D168" s="58"/>
-      <c r="E168" s="58"/>
-      <c r="F168" s="58"/>
-      <c r="G168" s="58"/>
-      <c r="H168" s="58"/>
-      <c r="I168" s="59"/>
-      <c r="J168" s="125"/>
-      <c r="K168" s="60"/>
+      <c r="A168" s="75" t="str">
+        <f>$A$124&amp;"."&amp;7</f>
+        <v>C.4.7</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
       <c r="L168" s="3"/>
     </row>
     <row r="169" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A169" s="9"/>
-      <c r="B169" s="58"/>
-      <c r="C169" s="58"/>
-      <c r="D169" s="58"/>
-      <c r="E169" s="58"/>
-      <c r="F169" s="58"/>
-      <c r="G169" s="58"/>
-      <c r="H169" s="58"/>
-      <c r="I169" s="59"/>
-      <c r="J169" s="125"/>
-      <c r="K169" s="60"/>
+      <c r="A169" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="11"/>
+      <c r="G169" s="11"/>
+      <c r="H169" s="11"/>
+      <c r="I169" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="J169" s="189">
+        <v>5.8831533524334558</v>
+      </c>
+      <c r="K169" s="93" t="s">
+        <v>85</v>
+      </c>
       <c r="L169" s="3"/>
     </row>
     <row r="170" spans="1:21" ht="20.100000000000001" customHeight="1">
@@ -36507,45 +36617,80 @@
       <c r="G174" s="58"/>
       <c r="H174" s="58"/>
       <c r="I174" s="59"/>
-      <c r="J174" s="63"/>
+      <c r="J174" s="125"/>
       <c r="K174" s="60"/>
       <c r="L174" s="3"/>
     </row>
     <row r="175" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A175" s="4"/>
-      <c r="B175" s="4"/>
-      <c r="C175" s="4"/>
-      <c r="D175" s="4"/>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
-      <c r="G175" s="4"/>
-      <c r="H175" s="4"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="58"/>
+      <c r="C175" s="58"/>
+      <c r="D175" s="58"/>
+      <c r="E175" s="58"/>
+      <c r="F175" s="58"/>
+      <c r="G175" s="58"/>
+      <c r="H175" s="58"/>
+      <c r="I175" s="59"/>
+      <c r="J175" s="125"/>
+      <c r="K175" s="60"/>
       <c r="L175" s="3"/>
     </row>
     <row r="176" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="4"/>
-      <c r="F176" s="4"/>
-      <c r="G176" s="4"/>
-      <c r="H176" s="4"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="4"/>
-      <c r="K176" s="4"/>
+      <c r="A176" s="9"/>
+      <c r="B176" s="58"/>
+      <c r="C176" s="58"/>
+      <c r="D176" s="58"/>
+      <c r="E176" s="58"/>
+      <c r="F176" s="58"/>
+      <c r="G176" s="58"/>
+      <c r="H176" s="58"/>
+      <c r="I176" s="59"/>
+      <c r="J176" s="63"/>
+      <c r="K176" s="60"/>
       <c r="L176" s="3"/>
     </row>
-    <row r="180" spans="2:4" ht="13.2">
-      <c r="B180" s="69"/>
-      <c r="C180" s="69"/>
-      <c r="D180" s="69"/>
+    <row r="177" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="3"/>
+    </row>
+    <row r="178" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="3"/>
+    </row>
+    <row r="182" spans="1:12" ht="13.2">
+      <c r="B182" s="69"/>
+      <c r="C182" s="69"/>
+      <c r="D182" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -36559,28 +36704,21 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="5" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="3" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="4" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="3" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -36603,11 +36741,11 @@
     <tabColor theme="0" tint="-0.249977111117893"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:DJ180"/>
+  <dimension ref="A1:DJ182"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A147" sqref="A147:XFD147"/>
+      <pane ySplit="1" topLeftCell="A159" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J169" sqref="J169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.100000000000001" customHeight="1" outlineLevelRow="1"/>
@@ -36693,12 +36831,12 @@
     </row>
     <row r="5" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A5" s="45"/>
-      <c r="B5" s="184"/>
-      <c r="C5" s="185"/>
-      <c r="D5" s="185"/>
-      <c r="E5" s="185"/>
-      <c r="F5" s="185"/>
-      <c r="G5" s="186"/>
+      <c r="B5" s="175"/>
+      <c r="C5" s="176"/>
+      <c r="D5" s="176"/>
+      <c r="E5" s="176"/>
+      <c r="F5" s="176"/>
+      <c r="G5" s="177"/>
       <c r="H5" s="44"/>
       <c r="I5" s="43"/>
       <c r="J5" s="43"/>
@@ -36706,12 +36844,12 @@
     </row>
     <row r="6" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A6" s="45"/>
-      <c r="B6" s="184"/>
-      <c r="C6" s="185"/>
-      <c r="D6" s="185"/>
-      <c r="E6" s="185"/>
-      <c r="F6" s="185"/>
-      <c r="G6" s="186"/>
+      <c r="B6" s="175"/>
+      <c r="C6" s="176"/>
+      <c r="D6" s="176"/>
+      <c r="E6" s="176"/>
+      <c r="F6" s="176"/>
+      <c r="G6" s="177"/>
       <c r="H6" s="44"/>
       <c r="I6" s="43"/>
       <c r="J6" s="43"/>
@@ -36719,12 +36857,12 @@
     </row>
     <row r="7" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A7" s="45"/>
-      <c r="B7" s="184"/>
-      <c r="C7" s="185"/>
-      <c r="D7" s="185"/>
-      <c r="E7" s="185"/>
-      <c r="F7" s="185"/>
-      <c r="G7" s="186"/>
+      <c r="B7" s="175"/>
+      <c r="C7" s="176"/>
+      <c r="D7" s="176"/>
+      <c r="E7" s="176"/>
+      <c r="F7" s="176"/>
+      <c r="G7" s="177"/>
       <c r="H7" s="44"/>
       <c r="I7" s="43"/>
       <c r="J7" s="43"/>
@@ -36732,12 +36870,12 @@
     </row>
     <row r="8" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A8" s="45"/>
-      <c r="B8" s="184"/>
-      <c r="C8" s="185"/>
-      <c r="D8" s="185"/>
-      <c r="E8" s="185"/>
-      <c r="F8" s="185"/>
-      <c r="G8" s="186"/>
+      <c r="B8" s="175"/>
+      <c r="C8" s="176"/>
+      <c r="D8" s="176"/>
+      <c r="E8" s="176"/>
+      <c r="F8" s="176"/>
+      <c r="G8" s="177"/>
       <c r="H8" s="44"/>
       <c r="I8" s="43"/>
       <c r="J8" s="43"/>
@@ -36745,12 +36883,12 @@
     </row>
     <row r="9" spans="1:15" s="41" customFormat="1" ht="20.100000000000001" hidden="1" customHeight="1" outlineLevel="1">
       <c r="A9" s="45"/>
-      <c r="B9" s="184"/>
-      <c r="C9" s="185"/>
-      <c r="D9" s="185"/>
-      <c r="E9" s="185"/>
-      <c r="F9" s="185"/>
-      <c r="G9" s="186"/>
+      <c r="B9" s="175"/>
+      <c r="C9" s="176"/>
+      <c r="D9" s="176"/>
+      <c r="E9" s="176"/>
+      <c r="F9" s="176"/>
+      <c r="G9" s="177"/>
       <c r="H9" s="44"/>
       <c r="I9" s="43"/>
       <c r="J9" s="43"/>
@@ -36798,117 +36936,117 @@
     </row>
     <row r="13" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A13" s="87"/>
-      <c r="B13" s="177" t="s">
+      <c r="B13" s="178" t="s">
         <v>100</v>
       </c>
-      <c r="C13" s="177"/>
-      <c r="D13" s="176" t="str">
+      <c r="C13" s="178"/>
+      <c r="D13" s="180" t="str">
         <f>PyFlange_Gap30deg!D13</f>
         <v>SP2200052</v>
       </c>
-      <c r="E13" s="176"/>
-      <c r="F13" s="176"/>
-      <c r="G13" s="176"/>
-      <c r="H13" s="176"/>
-      <c r="I13" s="176"/>
-      <c r="J13" s="176"/>
-      <c r="K13" s="176"/>
+      <c r="E13" s="180"/>
+      <c r="F13" s="180"/>
+      <c r="G13" s="180"/>
+      <c r="H13" s="180"/>
+      <c r="I13" s="180"/>
+      <c r="J13" s="180"/>
+      <c r="K13" s="180"/>
       <c r="L13" s="86"/>
     </row>
     <row r="14" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A14" s="87"/>
-      <c r="B14" s="177" t="s">
+      <c r="B14" s="178" t="s">
         <v>99</v>
       </c>
-      <c r="C14" s="177"/>
-      <c r="D14" s="176" t="str">
+      <c r="C14" s="178"/>
+      <c r="D14" s="180" t="str">
         <f>PyFlange_Gap30deg!D14</f>
         <v>Stichting GROW</v>
       </c>
-      <c r="E14" s="176"/>
-      <c r="F14" s="176"/>
-      <c r="G14" s="176"/>
-      <c r="H14" s="176"/>
-      <c r="I14" s="176"/>
-      <c r="J14" s="176"/>
-      <c r="K14" s="176"/>
+      <c r="E14" s="180"/>
+      <c r="F14" s="180"/>
+      <c r="G14" s="180"/>
+      <c r="H14" s="180"/>
+      <c r="I14" s="180"/>
+      <c r="J14" s="180"/>
+      <c r="K14" s="180"/>
       <c r="L14" s="86"/>
     </row>
     <row r="15" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A15" s="87"/>
-      <c r="B15" s="177" t="s">
+      <c r="B15" s="178" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="177"/>
-      <c r="D15" s="176" t="str">
+      <c r="C15" s="178"/>
+      <c r="D15" s="180" t="str">
         <f>PyFlange_Gap30deg!D15</f>
         <v>Bolt and Beautiful</v>
       </c>
-      <c r="E15" s="176"/>
-      <c r="F15" s="176"/>
-      <c r="G15" s="176"/>
-      <c r="H15" s="176"/>
-      <c r="I15" s="176"/>
-      <c r="J15" s="176"/>
-      <c r="K15" s="176"/>
+      <c r="E15" s="180"/>
+      <c r="F15" s="180"/>
+      <c r="G15" s="180"/>
+      <c r="H15" s="180"/>
+      <c r="I15" s="180"/>
+      <c r="J15" s="180"/>
+      <c r="K15" s="180"/>
       <c r="L15" s="86"/>
     </row>
     <row r="16" spans="1:15" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A16" s="87"/>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="178" t="s">
         <v>97</v>
       </c>
-      <c r="C16" s="177"/>
-      <c r="D16" s="176" t="str">
+      <c r="C16" s="178"/>
+      <c r="D16" s="180" t="str">
         <f>Title</f>
         <v>Flange Segment Analytical Model for 120° gap size</v>
       </c>
-      <c r="E16" s="176"/>
-      <c r="F16" s="176"/>
-      <c r="G16" s="176"/>
-      <c r="H16" s="176"/>
-      <c r="I16" s="176"/>
-      <c r="J16" s="176"/>
-      <c r="K16" s="176"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="180"/>
       <c r="L16" s="86"/>
       <c r="M16" s="88"/>
     </row>
     <row r="17" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A17" s="87"/>
-      <c r="B17" s="177" t="s">
+      <c r="B17" s="178" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="177"/>
-      <c r="D17" s="176" t="str">
+      <c r="C17" s="178"/>
+      <c r="D17" s="180" t="str">
         <f>PyFlange_Gap30deg!D17</f>
         <v>0.10</v>
       </c>
-      <c r="E17" s="176"/>
-      <c r="F17" s="176"/>
-      <c r="G17" s="176"/>
-      <c r="H17" s="176"/>
-      <c r="I17" s="176"/>
-      <c r="J17" s="176"/>
-      <c r="K17" s="176"/>
+      <c r="E17" s="180"/>
+      <c r="F17" s="180"/>
+      <c r="G17" s="180"/>
+      <c r="H17" s="180"/>
+      <c r="I17" s="180"/>
+      <c r="J17" s="180"/>
+      <c r="K17" s="180"/>
       <c r="L17" s="86"/>
     </row>
     <row r="18" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A18" s="87"/>
-      <c r="B18" s="177" t="s">
+      <c r="B18" s="178" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="177"/>
-      <c r="D18" s="187">
+      <c r="C18" s="178"/>
+      <c r="D18" s="179">
         <f>PyFlange_Gap30deg!D18</f>
         <v>45432</v>
       </c>
-      <c r="E18" s="187"/>
-      <c r="F18" s="187"/>
-      <c r="G18" s="187"/>
-      <c r="H18" s="187"/>
-      <c r="I18" s="187"/>
-      <c r="J18" s="187"/>
-      <c r="K18" s="187"/>
+      <c r="E18" s="179"/>
+      <c r="F18" s="179"/>
+      <c r="G18" s="179"/>
+      <c r="H18" s="179"/>
+      <c r="I18" s="179"/>
+      <c r="J18" s="179"/>
+      <c r="K18" s="179"/>
       <c r="L18" s="86"/>
     </row>
     <row r="19" spans="1:22" s="85" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
@@ -37096,16 +37234,16 @@
     </row>
     <row r="28" spans="1:22" s="18" customFormat="1" ht="20.100000000000001" customHeight="1" outlineLevel="1">
       <c r="A28" s="21"/>
-      <c r="B28" s="178"/>
-      <c r="C28" s="179"/>
-      <c r="D28" s="179"/>
-      <c r="E28" s="179"/>
-      <c r="F28" s="179"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="179"/>
-      <c r="I28" s="179"/>
-      <c r="J28" s="179"/>
-      <c r="K28" s="180"/>
+      <c r="B28" s="185"/>
+      <c r="C28" s="186"/>
+      <c r="D28" s="186"/>
+      <c r="E28" s="186"/>
+      <c r="F28" s="186"/>
+      <c r="G28" s="186"/>
+      <c r="H28" s="186"/>
+      <c r="I28" s="186"/>
+      <c r="J28" s="186"/>
+      <c r="K28" s="187"/>
       <c r="L28" s="20"/>
       <c r="M28" s="19"/>
       <c r="N28" s="19"/>
@@ -40899,31 +41037,46 @@
       <c r="L167" s="3"/>
     </row>
     <row r="168" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A168" s="9"/>
-      <c r="B168" s="58"/>
-      <c r="C168" s="58"/>
-      <c r="D168" s="58"/>
-      <c r="E168" s="58"/>
-      <c r="F168" s="58"/>
-      <c r="G168" s="58"/>
-      <c r="H168" s="58"/>
-      <c r="I168" s="59"/>
-      <c r="J168" s="125"/>
-      <c r="K168" s="60"/>
+      <c r="A168" s="75" t="str">
+        <f>$A$124&amp;"."&amp;7</f>
+        <v>D.4.7</v>
+      </c>
+      <c r="B168" s="12" t="s">
+        <v>413</v>
+      </c>
+      <c r="C168" s="12"/>
+      <c r="D168" s="12"/>
+      <c r="E168" s="12"/>
+      <c r="F168" s="12"/>
+      <c r="G168" s="12"/>
+      <c r="H168" s="12"/>
+      <c r="I168" s="12"/>
+      <c r="J168" s="12"/>
+      <c r="K168" s="12"/>
       <c r="L168" s="3"/>
     </row>
     <row r="169" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A169" s="9"/>
-      <c r="B169" s="58"/>
-      <c r="C169" s="58"/>
-      <c r="D169" s="58"/>
-      <c r="E169" s="58"/>
-      <c r="F169" s="58"/>
-      <c r="G169" s="58"/>
-      <c r="H169" s="58"/>
-      <c r="I169" s="59"/>
-      <c r="J169" s="125"/>
-      <c r="K169" s="60"/>
+      <c r="A169" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B169" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="C169" s="11"/>
+      <c r="D169" s="11"/>
+      <c r="E169" s="11"/>
+      <c r="F169" s="11"/>
+      <c r="G169" s="11"/>
+      <c r="H169" s="11"/>
+      <c r="I169" s="10" t="s">
+        <v>415</v>
+      </c>
+      <c r="J169" s="189">
+        <v>5.2371103182580327</v>
+      </c>
+      <c r="K169" s="93" t="s">
+        <v>85</v>
+      </c>
       <c r="L169" s="3"/>
     </row>
     <row r="170" spans="1:21" ht="20.100000000000001" customHeight="1">
@@ -40992,45 +41145,80 @@
       <c r="G174" s="58"/>
       <c r="H174" s="58"/>
       <c r="I174" s="59"/>
-      <c r="J174" s="63"/>
+      <c r="J174" s="125"/>
       <c r="K174" s="60"/>
       <c r="L174" s="3"/>
     </row>
     <row r="175" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A175" s="4"/>
-      <c r="B175" s="4"/>
-      <c r="C175" s="4"/>
-      <c r="D175" s="4"/>
-      <c r="E175" s="4"/>
-      <c r="F175" s="4"/>
-      <c r="G175" s="4"/>
-      <c r="H175" s="4"/>
-      <c r="I175" s="4"/>
-      <c r="J175" s="4"/>
-      <c r="K175" s="4"/>
+      <c r="A175" s="9"/>
+      <c r="B175" s="58"/>
+      <c r="C175" s="58"/>
+      <c r="D175" s="58"/>
+      <c r="E175" s="58"/>
+      <c r="F175" s="58"/>
+      <c r="G175" s="58"/>
+      <c r="H175" s="58"/>
+      <c r="I175" s="59"/>
+      <c r="J175" s="125"/>
+      <c r="K175" s="60"/>
       <c r="L175" s="3"/>
     </row>
     <row r="176" spans="1:21" ht="20.100000000000001" customHeight="1">
-      <c r="A176" s="4"/>
-      <c r="B176" s="4"/>
-      <c r="C176" s="4"/>
-      <c r="D176" s="4"/>
-      <c r="E176" s="4"/>
-      <c r="F176" s="4"/>
-      <c r="G176" s="4"/>
-      <c r="H176" s="4"/>
-      <c r="I176" s="4"/>
-      <c r="J176" s="4"/>
-      <c r="K176" s="4"/>
+      <c r="A176" s="9"/>
+      <c r="B176" s="58"/>
+      <c r="C176" s="58"/>
+      <c r="D176" s="58"/>
+      <c r="E176" s="58"/>
+      <c r="F176" s="58"/>
+      <c r="G176" s="58"/>
+      <c r="H176" s="58"/>
+      <c r="I176" s="59"/>
+      <c r="J176" s="63"/>
+      <c r="K176" s="60"/>
       <c r="L176" s="3"/>
     </row>
-    <row r="180" spans="2:4" ht="13.2">
-      <c r="B180" s="69"/>
-      <c r="C180" s="69"/>
-      <c r="D180" s="69"/>
+    <row r="177" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A177" s="4"/>
+      <c r="B177" s="4"/>
+      <c r="C177" s="4"/>
+      <c r="D177" s="4"/>
+      <c r="E177" s="4"/>
+      <c r="F177" s="4"/>
+      <c r="G177" s="4"/>
+      <c r="H177" s="4"/>
+      <c r="I177" s="4"/>
+      <c r="J177" s="4"/>
+      <c r="K177" s="4"/>
+      <c r="L177" s="3"/>
+    </row>
+    <row r="178" spans="1:12" ht="20.100000000000001" customHeight="1">
+      <c r="A178" s="4"/>
+      <c r="B178" s="4"/>
+      <c r="C178" s="4"/>
+      <c r="D178" s="4"/>
+      <c r="E178" s="4"/>
+      <c r="F178" s="4"/>
+      <c r="G178" s="4"/>
+      <c r="H178" s="4"/>
+      <c r="I178" s="4"/>
+      <c r="J178" s="4"/>
+      <c r="K178" s="4"/>
+      <c r="L178" s="3"/>
+    </row>
+    <row r="182" spans="1:12" ht="13.2">
+      <c r="B182" s="69"/>
+      <c r="C182" s="69"/>
+      <c r="D182" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="D16:K16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="D17:K17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="D18:K18"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="D15:K15"/>
     <mergeCell ref="A3:K3"/>
@@ -41044,28 +41232,21 @@
     <mergeCell ref="D13:K13"/>
     <mergeCell ref="B14:C14"/>
     <mergeCell ref="D14:K14"/>
-    <mergeCell ref="B28:K28"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="D16:K16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="D17:K17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="D18:K18"/>
   </mergeCells>
   <conditionalFormatting sqref="K64">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="3" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K94">
-    <cfRule type="cellIs" dxfId="1" priority="2" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="2" priority="2" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K124">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="1" stopIfTrue="1" operator="between">
       <formula>0</formula>
       <formula>1</formula>
     </cfRule>
@@ -41089,9 +41270,9 @@
   </sheetPr>
   <dimension ref="A1:AM1048558"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="26" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
+    <sheetView showGridLines="0" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="26" topLeftCell="A1193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
@@ -41741,7 +41922,7 @@
       <c r="P16" s="109">
         <v>0.78</v>
       </c>
-      <c r="U16" s="144">
+      <c r="U16" s="188">
         <v>2.1692199999999998E-2</v>
       </c>
       <c r="V16" s="144">
@@ -41956,10 +42137,10 @@
       <c r="J27" s="103" t="s">
         <v>196</v>
       </c>
-      <c r="L27" s="191"/>
-      <c r="M27" s="191"/>
-      <c r="N27" s="191"/>
-      <c r="O27" s="191"/>
+      <c r="L27" s="104"/>
+      <c r="M27" s="104"/>
+      <c r="N27" s="104"/>
+      <c r="O27" s="104"/>
       <c r="P27" t="str">
         <f t="shared" ref="P27:P66" si="2">IF(F27&lt;&gt;"",F27,"")</f>
         <v>Simplified formula used, therefore not evaluated</v>
@@ -42002,16 +42183,16 @@
       <c r="K28" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L28" s="192">
+      <c r="L28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="M28" s="192">
+      <c r="M28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="N28" s="192">
+      <c r="N28" s="107">
         <v>153.74071147146736</v>
       </c>
-      <c r="O28" s="192">
+      <c r="O28" s="107">
         <v>153.74071147146736</v>
       </c>
       <c r="P28" t="str">
@@ -42049,16 +42230,16 @@
       <c r="K29" s="103" t="s">
         <v>204</v>
       </c>
-      <c r="L29" s="192">
+      <c r="L29" s="107">
         <v>900</v>
       </c>
-      <c r="M29" s="192">
+      <c r="M29" s="107">
         <v>900</v>
       </c>
-      <c r="N29" s="192">
+      <c r="N29" s="107">
         <v>900</v>
       </c>
-      <c r="O29" s="192">
+      <c r="O29" s="107">
         <v>900</v>
       </c>
       <c r="P29" t="str">
@@ -42096,16 +42277,16 @@
       <c r="K30" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="L30" s="192">
+      <c r="L30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="M30" s="192">
+      <c r="M30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="N30" s="192">
+      <c r="N30" s="107">
         <v>4344.0716042398344</v>
       </c>
-      <c r="O30" s="192">
+      <c r="O30" s="107">
         <v>4344.0716042398344</v>
       </c>
       <c r="P30" t="str">
@@ -42149,16 +42330,16 @@
       <c r="K31" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L31" s="192">
+      <c r="L31" s="107">
         <v>2800</v>
       </c>
-      <c r="M31" s="192">
+      <c r="M31" s="107">
         <v>2800</v>
       </c>
-      <c r="N31" s="192">
+      <c r="N31" s="107">
         <v>2800</v>
       </c>
-      <c r="O31" s="192">
+      <c r="O31" s="107">
         <v>2800</v>
       </c>
       <c r="P31" t="str">
@@ -42196,16 +42377,16 @@
       <c r="K32" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L32" s="192">
+      <c r="L32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="M32" s="192">
+      <c r="M32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="N32" s="192">
+      <c r="N32" s="107">
         <v>3144.2390271487925</v>
       </c>
-      <c r="O32" s="192">
+      <c r="O32" s="107">
         <v>3144.2390271487925</v>
       </c>
       <c r="P32" t="str">
@@ -42243,16 +42424,16 @@
       <c r="K33" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L33" s="190">
+      <c r="L33" s="109">
         <v>0.03</v>
       </c>
-      <c r="M33" s="190">
+      <c r="M33" s="109">
         <v>0.03</v>
       </c>
-      <c r="N33" s="190">
+      <c r="N33" s="109">
         <v>0.03</v>
       </c>
-      <c r="O33" s="190">
+      <c r="O33" s="109">
         <v>0.03</v>
       </c>
       <c r="P33" t="str">
@@ -42291,16 +42472,16 @@
       <c r="K34" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L34" s="192">
+      <c r="L34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="M34" s="192">
+      <c r="M34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="N34" s="192">
+      <c r="N34" s="107">
         <v>3074.8142294293471</v>
       </c>
-      <c r="O34" s="192">
+      <c r="O34" s="107">
         <v>3074.8142294293471</v>
       </c>
       <c r="P34" t="str">
@@ -42346,16 +42527,16 @@
       <c r="K35" s="130" t="s">
         <v>127</v>
       </c>
-      <c r="L35" s="193">
-        <v>0</v>
-      </c>
-      <c r="M35" s="193">
-        <v>0</v>
-      </c>
-      <c r="N35" s="193">
-        <v>0</v>
-      </c>
-      <c r="O35" s="193">
+      <c r="L35" s="129">
+        <v>0</v>
+      </c>
+      <c r="M35" s="129">
+        <v>0</v>
+      </c>
+      <c r="N35" s="129">
+        <v>0</v>
+      </c>
+      <c r="O35" s="129">
         <v>0</v>
       </c>
       <c r="P35" t="str">
@@ -42390,16 +42571,16 @@
       <c r="K36" s="103" t="s">
         <v>274</v>
       </c>
-      <c r="L36" s="194">
+      <c r="L36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="M36" s="194">
+      <c r="M36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="N36" s="194">
+      <c r="N36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
-      <c r="O36" s="194">
+      <c r="O36" s="114">
         <v>5.8458922294713925E-10</v>
       </c>
       <c r="P36" t="str">
@@ -42435,16 +42616,16 @@
       <c r="K37" s="103" t="s">
         <v>274</v>
       </c>
-      <c r="L37" s="194">
+      <c r="L37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="M37" s="194">
+      <c r="M37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="N37" s="194">
+      <c r="N37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
-      <c r="O37" s="194">
+      <c r="O37" s="114">
         <v>9.6993208304588435E-11</v>
       </c>
       <c r="P37" t="str">
@@ -42479,16 +42660,16 @@
       <c r="K38" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L38" s="190">
+      <c r="L38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="M38" s="190">
+      <c r="M38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="N38" s="190">
+      <c r="N38" s="109">
         <v>0.1423059102718657</v>
       </c>
-      <c r="O38" s="190">
+      <c r="O38" s="109">
         <v>0.1423059102718657</v>
       </c>
       <c r="P38" t="str">
@@ -42529,16 +42710,16 @@
       <c r="K39" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L39" s="189">
+      <c r="L39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="M39" s="189">
+      <c r="M39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="N39" s="189">
+      <c r="N39" s="108">
         <v>48.860015706266829</v>
       </c>
-      <c r="O39" s="189">
+      <c r="O39" s="108">
         <v>48.860015706266829</v>
       </c>
       <c r="P39" t="str">
@@ -42573,16 +42754,16 @@
       <c r="K40" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="L40" s="192">
+      <c r="L40" s="107">
         <v>500</v>
       </c>
-      <c r="M40" s="192">
+      <c r="M40" s="107">
         <v>500</v>
       </c>
-      <c r="N40" s="192">
+      <c r="N40" s="107">
         <v>500</v>
       </c>
-      <c r="O40" s="192">
+      <c r="O40" s="107">
         <v>500</v>
       </c>
       <c r="P40" t="str">
@@ -42626,16 +42807,16 @@
       <c r="K41" s="103" t="s">
         <v>273</v>
       </c>
-      <c r="L41" s="192">
+      <c r="L41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="M41" s="192">
+      <c r="M41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="N41" s="192">
+      <c r="N41" s="107">
         <v>33.30212829607494</v>
       </c>
-      <c r="O41" s="192">
+      <c r="O41" s="107">
         <v>33.30212829607494</v>
       </c>
       <c r="P41" t="str">
@@ -42676,16 +42857,16 @@
       <c r="K42" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L42" s="195">
+      <c r="L42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="M42" s="195">
+      <c r="M42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="N42" s="195">
+      <c r="N42" s="111">
         <v>3323.2147772434732</v>
       </c>
-      <c r="O42" s="195">
+      <c r="O42" s="111">
         <v>3323.2147772434732</v>
       </c>
       <c r="P42" t="str">
@@ -42730,16 +42911,16 @@
       <c r="K43" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="L43" s="192">
+      <c r="L43" s="107">
         <v>314.32350000000002</v>
       </c>
-      <c r="M43" s="192">
+      <c r="M43" s="107">
         <v>314.32350000000002</v>
       </c>
-      <c r="N43" s="192">
+      <c r="N43" s="107">
         <v>314.32350000000002</v>
       </c>
-      <c r="O43" s="192">
+      <c r="O43" s="107">
         <v>314.32350000000002</v>
       </c>
       <c r="P43" t="str">
@@ -42780,16 +42961,16 @@
       <c r="K44" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="L44" s="192">
+      <c r="L44" s="107">
         <v>314.32350000000002</v>
       </c>
-      <c r="M44" s="192">
+      <c r="M44" s="107">
         <v>314.32350000000002</v>
       </c>
-      <c r="N44" s="192">
+      <c r="N44" s="107">
         <v>314.32350000000002</v>
       </c>
-      <c r="O44" s="192">
+      <c r="O44" s="107">
         <v>314.32350000000002</v>
       </c>
       <c r="P44" t="str">
@@ -42830,16 +43011,16 @@
       <c r="K45" s="103" t="s">
         <v>182</v>
       </c>
-      <c r="L45" s="192">
+      <c r="L45" s="107">
         <v>-294.16150000000005</v>
       </c>
-      <c r="M45" s="192">
+      <c r="M45" s="107">
         <v>-294.16150000000005</v>
       </c>
-      <c r="N45" s="192">
+      <c r="N45" s="107">
         <v>-294.16150000000005</v>
       </c>
-      <c r="O45" s="192">
+      <c r="O45" s="107">
         <v>-294.16150000000005</v>
       </c>
       <c r="P45" t="str">
@@ -42874,16 +43055,16 @@
       <c r="K46" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L46" s="195">
+      <c r="L46" s="111">
         <v>1287.1661307088773</v>
       </c>
-      <c r="M46" s="195">
+      <c r="M46" s="111">
         <v>1287.1661307088773</v>
       </c>
-      <c r="N46" s="195">
+      <c r="N46" s="111">
         <v>1287.1661307088773</v>
       </c>
-      <c r="O46" s="195">
+      <c r="O46" s="111">
         <v>1287.1661307088773</v>
       </c>
       <c r="P46" t="str">
@@ -42925,10 +43106,10 @@
       <c r="K47" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L47" s="191"/>
-      <c r="M47" s="191"/>
-      <c r="N47" s="191"/>
-      <c r="O47" s="191"/>
+      <c r="L47" s="104"/>
+      <c r="M47" s="104"/>
+      <c r="N47" s="104"/>
+      <c r="O47" s="104"/>
       <c r="P47" t="str">
         <f t="shared" si="2"/>
         <v>(valid in case L-Flange is calculated)</v>
@@ -42961,16 +43142,16 @@
       <c r="K48" s="103" t="s">
         <v>178</v>
       </c>
-      <c r="L48" s="188">
+      <c r="L48" s="110">
         <v>30</v>
       </c>
-      <c r="M48" s="188">
+      <c r="M48" s="110">
         <v>60</v>
       </c>
-      <c r="N48" s="188">
+      <c r="N48" s="110">
         <v>90</v>
       </c>
-      <c r="O48" s="188">
+      <c r="O48" s="110">
         <v>120</v>
       </c>
       <c r="P48" t="str">
@@ -43008,16 +43189,16 @@
       <c r="K49" s="103" t="s">
         <v>171</v>
       </c>
-      <c r="L49" s="190">
+      <c r="L49" s="109">
         <v>1.9634954084936207</v>
       </c>
-      <c r="M49" s="190">
+      <c r="M49" s="109">
         <v>3.9269908169872414</v>
       </c>
-      <c r="N49" s="190">
+      <c r="N49" s="109">
         <v>5.8904862254808625</v>
       </c>
-      <c r="O49" s="190">
+      <c r="O49" s="109">
         <v>7.8539816339744828</v>
       </c>
       <c r="P49" t="str">
@@ -43052,16 +43233,16 @@
       <c r="K50" s="103" t="s">
         <v>171</v>
       </c>
-      <c r="L50" s="190">
+      <c r="L50" s="109">
         <v>7.5</v>
       </c>
-      <c r="M50" s="190">
+      <c r="M50" s="109">
         <v>7.5</v>
       </c>
-      <c r="N50" s="190">
+      <c r="N50" s="109">
         <v>7.5</v>
       </c>
-      <c r="O50" s="190">
+      <c r="O50" s="109">
         <v>7.5</v>
       </c>
       <c r="P50" t="str">
@@ -43096,16 +43277,16 @@
       <c r="K51" s="103" t="s">
         <v>175</v>
       </c>
-      <c r="L51" s="189">
+      <c r="L51" s="108">
         <v>1.4</v>
       </c>
-      <c r="M51" s="189">
+      <c r="M51" s="108">
         <v>1.4</v>
       </c>
-      <c r="N51" s="189">
+      <c r="N51" s="108">
         <v>1.4</v>
       </c>
-      <c r="O51" s="189">
+      <c r="O51" s="108">
         <v>1.4</v>
       </c>
       <c r="P51" t="str">
@@ -43146,16 +43327,16 @@
       <c r="K52" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L52" s="190">
+      <c r="L52" s="109">
         <v>0.28773533056547307</v>
       </c>
-      <c r="M52" s="190">
+      <c r="M52" s="109">
         <v>0.74253427729521915</v>
       </c>
-      <c r="N52" s="190">
+      <c r="N52" s="109">
         <v>1.3643968401892383</v>
       </c>
-      <c r="O52" s="190">
+      <c r="O52" s="109">
         <v>2.1533230192475301</v>
       </c>
       <c r="P52" t="str">
@@ -43197,16 +43378,16 @@
       <c r="K53" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L53" s="190">
+      <c r="L53" s="109">
         <v>1.2162355202035975</v>
       </c>
-      <c r="M53" s="190">
+      <c r="M53" s="109">
         <v>0.63575115537527993</v>
       </c>
-      <c r="N53" s="190">
+      <c r="N53" s="109">
         <v>0.4993626397773579</v>
       </c>
-      <c r="O53" s="190">
+      <c r="O53" s="109">
         <v>0.44426272750754409</v>
       </c>
       <c r="P53" t="str">
@@ -43242,16 +43423,16 @@
       <c r="K54" s="103" t="s">
         <v>171</v>
       </c>
-      <c r="L54" s="190">
+      <c r="L54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="M54" s="190">
+      <c r="M54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="N54" s="190">
+      <c r="N54" s="109">
         <v>1.9634954084936205</v>
       </c>
-      <c r="O54" s="190">
+      <c r="O54" s="109">
         <v>1.9634954084936205</v>
       </c>
       <c r="P54" t="str">
@@ -43293,16 +43474,16 @@
       <c r="K55" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L55" s="190">
+      <c r="L55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="M55" s="190">
+      <c r="M55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="N55" s="190">
+      <c r="N55" s="109">
         <v>1.9617469257392748</v>
       </c>
-      <c r="O55" s="190">
+      <c r="O55" s="109">
         <v>1.9617469257392748</v>
       </c>
       <c r="P55" t="str">
@@ -43344,16 +43525,16 @@
       <c r="K56" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L56" s="190">
+      <c r="L56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="M56" s="190">
+      <c r="M56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="N56" s="190">
+      <c r="N56" s="109">
         <v>2.942620388608912</v>
       </c>
-      <c r="O56" s="190">
+      <c r="O56" s="109">
         <v>2.942620388608912</v>
       </c>
       <c r="P56" t="str">
@@ -43391,16 +43572,16 @@
         <v>168</v>
       </c>
       <c r="K57" s="103"/>
-      <c r="L57" s="190">
+      <c r="L57" s="109">
         <v>0.95286282352314688</v>
       </c>
-      <c r="M57" s="190">
+      <c r="M57" s="109">
         <v>0.58262609700472079</v>
       </c>
-      <c r="N57" s="190">
+      <c r="N57" s="109">
         <v>0.47184092472685457</v>
       </c>
-      <c r="O57" s="190">
+      <c r="O57" s="109">
         <v>0.42441366570439232</v>
       </c>
       <c r="P57" t="str">
@@ -43438,16 +43619,16 @@
         <v>167</v>
       </c>
       <c r="K58" s="103"/>
-      <c r="L58" s="190">
+      <c r="L58" s="109">
         <v>-1.6996879926957522</v>
       </c>
-      <c r="M58" s="190">
+      <c r="M58" s="109">
         <v>-0.46741282911895099</v>
       </c>
-      <c r="N58" s="190">
+      <c r="N58" s="109">
         <v>0.19939552653846943</v>
       </c>
-      <c r="O58" s="190">
+      <c r="O58" s="109">
         <v>0.67694875947348121</v>
       </c>
       <c r="P58" t="str">
@@ -43485,16 +43666,16 @@
         <v>166</v>
       </c>
       <c r="K59" s="103"/>
-      <c r="L59" s="190">
+      <c r="L59" s="109">
         <v>-0.13232393428252798</v>
       </c>
-      <c r="M59" s="190">
+      <c r="M59" s="109">
         <v>0.49094883784411425</v>
       </c>
-      <c r="N59" s="190">
+      <c r="N59" s="109">
         <v>0.97552666362167262</v>
       </c>
-      <c r="O59" s="190">
+      <c r="O59" s="109">
         <v>1.3750667981906362</v>
       </c>
       <c r="P59" t="str">
@@ -43535,16 +43716,16 @@
       <c r="K60" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L60" s="190">
+      <c r="L60" s="109">
         <v>0.87601845454409977</v>
       </c>
-      <c r="M60" s="190">
+      <c r="M60" s="109">
         <v>1.6338216149415525</v>
       </c>
-      <c r="N60" s="190">
+      <c r="N60" s="109">
         <v>2.6525058127308667</v>
       </c>
-      <c r="O60" s="190">
+      <c r="O60" s="109">
         <v>3.9552630780086151</v>
       </c>
       <c r="P60" t="str">
@@ -43582,16 +43763,16 @@
       <c r="K61" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L61" s="190">
+      <c r="L61" s="109">
         <v>0.87601845454409977</v>
       </c>
-      <c r="M61" s="190">
+      <c r="M61" s="109">
         <v>1.6338216149415525</v>
       </c>
-      <c r="N61" s="190">
+      <c r="N61" s="109">
         <v>2.6525058127308667</v>
       </c>
-      <c r="O61" s="190">
+      <c r="O61" s="109">
         <v>3.9552630780086151</v>
       </c>
       <c r="P61" t="str">
@@ -43629,10 +43810,10 @@
         <v>162</v>
       </c>
       <c r="K62" s="103"/>
-      <c r="L62" s="196"/>
-      <c r="M62" s="196"/>
-      <c r="N62" s="196"/>
-      <c r="O62" s="196"/>
+      <c r="L62" s="128"/>
+      <c r="M62" s="128"/>
+      <c r="N62" s="128"/>
+      <c r="O62" s="128"/>
       <c r="P62" t="str">
         <f t="shared" si="2"/>
         <v>Gap shape formula</v>
@@ -43668,10 +43849,10 @@
         <v>160</v>
       </c>
       <c r="K63" s="103"/>
-      <c r="L63" s="196"/>
-      <c r="M63" s="196"/>
-      <c r="N63" s="196"/>
-      <c r="O63" s="196"/>
+      <c r="L63" s="128"/>
+      <c r="M63" s="128"/>
+      <c r="N63" s="128"/>
+      <c r="O63" s="128"/>
       <c r="P63" t="str">
         <f t="shared" si="2"/>
         <v>Stress range formula</v>
@@ -43704,10 +43885,10 @@
         <v>158</v>
       </c>
       <c r="K64" s="103"/>
-      <c r="L64" s="191"/>
-      <c r="M64" s="191"/>
-      <c r="N64" s="191"/>
-      <c r="O64" s="191"/>
+      <c r="L64" s="104"/>
+      <c r="M64" s="104"/>
+      <c r="N64" s="104"/>
+      <c r="O64" s="104"/>
       <c r="P64" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -43740,10 +43921,10 @@
         <v>157</v>
       </c>
       <c r="K65" s="103"/>
-      <c r="L65" s="191"/>
-      <c r="M65" s="191"/>
-      <c r="N65" s="191"/>
-      <c r="O65" s="191"/>
+      <c r="L65" s="104"/>
+      <c r="M65" s="104"/>
+      <c r="N65" s="104"/>
+      <c r="O65" s="104"/>
       <c r="P65" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -43779,10 +43960,10 @@
         <v>156</v>
       </c>
       <c r="K66" s="103"/>
-      <c r="L66" s="196"/>
-      <c r="M66" s="196"/>
-      <c r="N66" s="196"/>
-      <c r="O66" s="196"/>
+      <c r="L66" s="128"/>
+      <c r="M66" s="128"/>
+      <c r="N66" s="128"/>
+      <c r="O66" s="128"/>
       <c r="P66" t="str">
         <f t="shared" si="2"/>
         <v>Summarized formula for bolt force curve</v>
@@ -43815,16 +43996,16 @@
       <c r="K67" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L67" s="190">
+      <c r="L67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="M67" s="190">
+      <c r="M67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="N67" s="190">
+      <c r="N67" s="109">
         <v>-123.29166666666667</v>
       </c>
-      <c r="O67" s="190">
+      <c r="O67" s="109">
         <v>-123.29166666666667</v>
       </c>
       <c r="U67" s="144">
@@ -43855,16 +44036,16 @@
       <c r="K68" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L68" s="190">
+      <c r="L68" s="109">
         <v>2800</v>
       </c>
-      <c r="M68" s="190">
+      <c r="M68" s="109">
         <v>2800</v>
       </c>
-      <c r="N68" s="190">
+      <c r="N68" s="109">
         <v>2800</v>
       </c>
-      <c r="O68" s="190">
+      <c r="O68" s="109">
         <v>2800</v>
       </c>
       <c r="U68" s="144">
@@ -43895,16 +44076,16 @@
       <c r="K69" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L69" s="190">
+      <c r="L69" s="109">
         <v>1909.4309784365259</v>
       </c>
-      <c r="M69" s="190">
+      <c r="M69" s="109">
         <v>1690.9555902310638</v>
       </c>
-      <c r="N69" s="190">
+      <c r="N69" s="109">
         <v>1538.0236675777603</v>
       </c>
-      <c r="O69" s="190">
+      <c r="O69" s="109">
         <v>1569.3540427928758</v>
       </c>
       <c r="U69" s="144">
@@ -43935,16 +44116,16 @@
       <c r="K70" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L70" s="190">
+      <c r="L70" s="109">
         <v>3500</v>
       </c>
-      <c r="M70" s="190">
+      <c r="M70" s="109">
         <v>3500</v>
       </c>
-      <c r="N70" s="190">
+      <c r="N70" s="109">
         <v>3500</v>
       </c>
-      <c r="O70" s="190">
+      <c r="O70" s="109">
         <v>3500</v>
       </c>
       <c r="U70" s="144">
@@ -43975,16 +44156,16 @@
       <c r="K71" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L71" s="190">
+      <c r="L71" s="109">
         <v>156.76717506300358</v>
       </c>
-      <c r="M71" s="190">
+      <c r="M71" s="109">
         <v>126.00313799480629</v>
       </c>
-      <c r="N71" s="190">
+      <c r="N71" s="109">
         <v>116.91912725921244</v>
       </c>
-      <c r="O71" s="190">
+      <c r="O71" s="109">
         <v>109.76791994954699</v>
       </c>
       <c r="U71" s="144">
@@ -44015,16 +44196,16 @@
       <c r="K72" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L72" s="190">
+      <c r="L72" s="109">
         <v>2822.4201487344362</v>
       </c>
-      <c r="M72" s="190">
+      <c r="M72" s="109">
         <v>2816.7929652634075</v>
       </c>
-      <c r="N72" s="190">
+      <c r="N72" s="109">
         <v>2816.8335832950702</v>
       </c>
-      <c r="O72" s="190">
+      <c r="O72" s="109">
         <v>2813.6067292949529</v>
       </c>
       <c r="U72" s="144">
@@ -44051,16 +44232,16 @@
         <v>312</v>
       </c>
       <c r="K73" s="103"/>
-      <c r="L73" s="188">
+      <c r="L73" s="110">
         <v>997759866.88190949</v>
       </c>
-      <c r="M73" s="188">
+      <c r="M73" s="110">
         <v>707800475.26499701</v>
       </c>
-      <c r="N73" s="188">
+      <c r="N73" s="110">
         <v>567114327.41726518</v>
       </c>
-      <c r="O73" s="188">
+      <c r="O73" s="110">
         <v>575788202.34221888</v>
       </c>
       <c r="U73" s="144">
@@ -44087,16 +44268,16 @@
         <v>311</v>
       </c>
       <c r="K74" s="103"/>
-      <c r="L74" s="195">
+      <c r="L74" s="111">
         <v>150467.24517169897</v>
       </c>
-      <c r="M74" s="195">
+      <c r="M74" s="111">
         <v>144039.77209871516</v>
       </c>
-      <c r="N74" s="195">
+      <c r="N74" s="111">
         <v>140181.66568973445</v>
       </c>
-      <c r="O74" s="195">
+      <c r="O74" s="111">
         <v>140110.33867047014</v>
       </c>
       <c r="U74" s="144">
@@ -44123,16 +44304,16 @@
         <v>310</v>
       </c>
       <c r="K75" s="103"/>
-      <c r="L75" s="195">
+      <c r="L75" s="111">
         <v>74838834.565129951</v>
       </c>
-      <c r="M75" s="195">
+      <c r="M75" s="111">
         <v>47288206.841718264</v>
       </c>
-      <c r="N75" s="195">
+      <c r="N75" s="111">
         <v>40635766.52482488</v>
       </c>
-      <c r="O75" s="195">
+      <c r="O75" s="111">
         <v>35511087.636771843</v>
       </c>
       <c r="U75" s="144">
@@ -44159,16 +44340,16 @@
         <v>309</v>
       </c>
       <c r="K76" s="103"/>
-      <c r="L76" s="198">
+      <c r="L76" s="136">
         <v>1.5080506860024631E-4</v>
       </c>
-      <c r="M76" s="198">
+      <c r="M76" s="136">
         <v>2.0350335600550053E-4</v>
       </c>
-      <c r="N76" s="198">
+      <c r="N76" s="136">
         <v>2.4718413715298912E-4</v>
       </c>
-      <c r="O76" s="198">
+      <c r="O76" s="136">
         <v>2.4333659165040649E-4</v>
       </c>
       <c r="U76" s="144">
@@ -44195,16 +44376,16 @@
         <v>308</v>
       </c>
       <c r="K77" s="103"/>
-      <c r="L77" s="198">
+      <c r="L77" s="136">
         <v>7.5006859916112015E-2</v>
       </c>
-      <c r="M77" s="198">
+      <c r="M77" s="136">
         <v>6.6810080657283805E-2</v>
       </c>
-      <c r="N77" s="198">
+      <c r="N77" s="136">
         <v>7.1653570647539536E-2</v>
       </c>
-      <c r="O77" s="198">
+      <c r="O77" s="136">
         <v>6.1673871559573705E-2</v>
       </c>
       <c r="U77" s="144">
@@ -44231,16 +44412,16 @@
         <v>307</v>
       </c>
       <c r="K78" s="103"/>
-      <c r="L78" s="189">
+      <c r="L78" s="108">
         <v>2806.9553577950619</v>
       </c>
-      <c r="M78" s="189">
+      <c r="M78" s="108">
         <v>2805.1437052436527</v>
       </c>
-      <c r="N78" s="189">
+      <c r="N78" s="108">
         <v>2805.0768828471073</v>
       </c>
-      <c r="O78" s="189">
+      <c r="O78" s="108">
         <v>2803.9049550183272</v>
       </c>
       <c r="U78" s="144">
@@ -44277,16 +44458,16 @@
       <c r="K79" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L79" s="192">
+      <c r="L79" s="107">
         <v>787.57931096911932</v>
       </c>
-      <c r="M79" s="192">
+      <c r="M79" s="107">
         <v>662.70349320710886</v>
       </c>
-      <c r="N79" s="192">
+      <c r="N79" s="107">
         <v>689.42837161335797</v>
       </c>
-      <c r="O79" s="192">
+      <c r="O79" s="107">
         <v>574.37016229170865</v>
       </c>
       <c r="P79" t="str">
@@ -44321,16 +44502,16 @@
       <c r="K80" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="L80" s="195">
+      <c r="L80" s="111">
         <v>38818.827824694483</v>
       </c>
-      <c r="M80" s="195">
+      <c r="M80" s="111">
         <v>38818.827824694483</v>
       </c>
-      <c r="N80" s="195">
+      <c r="N80" s="111">
         <v>38818.827824694483</v>
       </c>
-      <c r="O80" s="195">
+      <c r="O80" s="111">
         <v>38818.827824694483</v>
       </c>
       <c r="P80" t="str">
@@ -44365,16 +44546,16 @@
       <c r="K81" s="103" t="s">
         <v>272</v>
       </c>
-      <c r="L81" s="199">
+      <c r="L81" s="135">
         <v>129396092.74898161</v>
       </c>
-      <c r="M81" s="199">
+      <c r="M81" s="135">
         <v>129396092.74898161</v>
       </c>
-      <c r="N81" s="199">
+      <c r="N81" s="135">
         <v>129396092.74898161</v>
       </c>
-      <c r="O81" s="199">
+      <c r="O81" s="135">
         <v>129396092.74898161</v>
       </c>
       <c r="P81" t="str">
@@ -44409,16 +44590,16 @@
       <c r="K82" s="103" t="s">
         <v>142</v>
       </c>
-      <c r="L82" s="195">
+      <c r="L82" s="111">
         <v>86999.999999999971</v>
       </c>
-      <c r="M82" s="195">
+      <c r="M82" s="111">
         <v>86999.999999999971</v>
       </c>
-      <c r="N82" s="195">
+      <c r="N82" s="111">
         <v>86999.999999999971</v>
       </c>
-      <c r="O82" s="195">
+      <c r="O82" s="111">
         <v>86999.999999999971</v>
       </c>
       <c r="P82" t="str">
@@ -44453,16 +44634,16 @@
       <c r="K83" s="103" t="s">
         <v>272</v>
       </c>
-      <c r="L83" s="199">
+      <c r="L83" s="135">
         <v>289999999.99999994</v>
       </c>
-      <c r="M83" s="199">
+      <c r="M83" s="135">
         <v>289999999.99999994</v>
       </c>
-      <c r="N83" s="199">
+      <c r="N83" s="135">
         <v>289999999.99999994</v>
       </c>
-      <c r="O83" s="199">
+      <c r="O83" s="135">
         <v>289999999.99999994</v>
       </c>
       <c r="P83" t="str">
@@ -44503,16 +44684,16 @@
       <c r="K84" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="L84" s="195">
+      <c r="L84" s="111">
         <v>9264.0015244499918</v>
       </c>
-      <c r="M84" s="195">
+      <c r="M84" s="111">
         <v>4179.5757097437345</v>
       </c>
-      <c r="N84" s="195">
+      <c r="N84" s="111">
         <v>2678.2454850162208</v>
       </c>
-      <c r="O84" s="195">
+      <c r="O84" s="111">
         <v>1496.3530379691292</v>
       </c>
       <c r="P84" t="str">
@@ -44547,16 +44728,16 @@
       <c r="K85" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L85" s="189">
+      <c r="L85" s="108">
         <v>1.5</v>
       </c>
-      <c r="M85" s="189">
+      <c r="M85" s="108">
         <v>2</v>
       </c>
-      <c r="N85" s="189">
+      <c r="N85" s="108">
         <v>2.5</v>
       </c>
-      <c r="O85" s="189">
+      <c r="O85" s="108">
         <v>2.5</v>
       </c>
       <c r="U85" s="144">
@@ -44596,16 +44777,16 @@
       <c r="K86" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="L86" s="195">
+      <c r="L86" s="111">
         <v>4755.8743101826412</v>
       </c>
-      <c r="M86" s="195">
+      <c r="M86" s="111">
         <v>1994.0356568620355</v>
       </c>
-      <c r="N86" s="195">
+      <c r="N86" s="111">
         <v>1052.1040815198671</v>
       </c>
-      <c r="O86" s="195">
+      <c r="O86" s="111">
         <v>592.43643599938059</v>
       </c>
       <c r="P86" t="str">
@@ -44643,16 +44824,16 @@
       <c r="K87" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="L87" s="195">
+      <c r="L87" s="111">
         <v>5118.8473830169332</v>
       </c>
-      <c r="M87" s="195">
+      <c r="M87" s="111">
         <v>2209.1525376668401</v>
       </c>
-      <c r="N87" s="195">
+      <c r="N87" s="111">
         <v>1239.3817215558724</v>
       </c>
-      <c r="O87" s="195">
+      <c r="O87" s="111">
         <v>802.38409839730571</v>
       </c>
       <c r="P87" t="str">
@@ -44690,16 +44871,16 @@
       <c r="K88" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="L88" s="195">
+      <c r="L88" s="111">
         <v>4755.8743101826412</v>
       </c>
-      <c r="M88" s="195">
+      <c r="M88" s="111">
         <v>1994.0356568620355</v>
       </c>
-      <c r="N88" s="195">
+      <c r="N88" s="111">
         <v>1052.1040815198671</v>
       </c>
-      <c r="O88" s="195">
+      <c r="O88" s="111">
         <v>592.43643599938059</v>
       </c>
       <c r="P88" t="str">
@@ -44740,16 +44921,16 @@
       <c r="K89" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L89" s="190">
+      <c r="L89" s="109">
         <v>1.8</v>
       </c>
-      <c r="M89" s="190">
+      <c r="M89" s="109">
         <v>2.0853981633974481</v>
       </c>
-      <c r="N89" s="190">
+      <c r="N89" s="109">
         <v>2.4780972450961727</v>
       </c>
-      <c r="O89" s="190">
+      <c r="O89" s="109">
         <v>2.8707963267948964</v>
       </c>
       <c r="P89" t="str">
@@ -44790,16 +44971,16 @@
       <c r="K90" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="L90" s="192">
+      <c r="L90" s="107">
         <v>1420.1267061173535</v>
       </c>
-      <c r="M90" s="192">
+      <c r="M90" s="107">
         <v>95.752198009831744</v>
       </c>
-      <c r="N90" s="192">
+      <c r="N90" s="107">
         <v>19.194112486621194</v>
       </c>
-      <c r="O90" s="192">
+      <c r="O90" s="107">
         <v>6.1047791882710731</v>
       </c>
       <c r="P90" t="str">
@@ -44843,16 +45024,16 @@
       <c r="K91" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L91" s="192">
+      <c r="L91" s="107">
         <v>537.29586434313285</v>
       </c>
-      <c r="M91" s="192">
+      <c r="M91" s="107">
         <v>561.15079343168679</v>
       </c>
-      <c r="N91" s="192">
+      <c r="N91" s="107">
         <v>569.99792927094325</v>
       </c>
-      <c r="O91" s="192">
+      <c r="O91" s="107">
         <v>578.80131521362864</v>
       </c>
       <c r="P91" t="str">
@@ -44896,16 +45077,16 @@
       <c r="K92" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L92" s="192">
+      <c r="L92" s="107">
         <v>408.30868419464207</v>
       </c>
-      <c r="M92" s="192">
+      <c r="M92" s="107">
         <v>302.12207356439359</v>
       </c>
-      <c r="N92" s="192">
+      <c r="N92" s="107">
         <v>262.74038581891148</v>
       </c>
-      <c r="O92" s="192">
+      <c r="O92" s="107">
         <v>223.55344412423759</v>
       </c>
       <c r="P92" t="str">
@@ -44943,16 +45124,16 @@
       <c r="K93" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L93" s="189">
-        <v>0</v>
-      </c>
-      <c r="M93" s="189">
-        <v>0</v>
-      </c>
-      <c r="N93" s="189">
-        <v>0</v>
-      </c>
-      <c r="O93" s="189">
+      <c r="L93" s="108">
+        <v>0</v>
+      </c>
+      <c r="M93" s="108">
+        <v>0</v>
+      </c>
+      <c r="N93" s="108">
+        <v>0</v>
+      </c>
+      <c r="O93" s="108">
         <v>0</v>
       </c>
       <c r="P93" t="str">
@@ -44993,16 +45174,16 @@
       <c r="K94" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L94" s="192">
+      <c r="L94" s="107">
         <v>787.57931096911932</v>
       </c>
-      <c r="M94" s="192">
+      <c r="M94" s="107">
         <v>662.70349320710886</v>
       </c>
-      <c r="N94" s="192">
+      <c r="N94" s="107">
         <v>689.42837161335797</v>
       </c>
-      <c r="O94" s="192">
+      <c r="O94" s="107">
         <v>574.37016229170865</v>
       </c>
       <c r="P94" t="str">
@@ -45043,16 +45224,16 @@
       <c r="K95" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L95" s="192">
+      <c r="L95" s="107">
         <v>3500</v>
       </c>
-      <c r="M95" s="192">
+      <c r="M95" s="107">
         <v>3500</v>
       </c>
-      <c r="N95" s="192">
+      <c r="N95" s="107">
         <v>3500</v>
       </c>
-      <c r="O95" s="192">
+      <c r="O95" s="107">
         <v>3500</v>
       </c>
       <c r="P95" t="str">
@@ -45096,16 +45277,16 @@
       <c r="K96" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L96" s="192">
+      <c r="L96" s="107">
         <v>2014.2804877190592</v>
       </c>
-      <c r="M96" s="192">
+      <c r="M96" s="107">
         <v>2014.2804877190592</v>
       </c>
-      <c r="N96" s="192">
+      <c r="N96" s="107">
         <v>2014.2804877190592</v>
       </c>
-      <c r="O96" s="192">
+      <c r="O96" s="107">
         <v>2014.2804877190592</v>
       </c>
       <c r="P96" t="str">
@@ -45149,16 +45330,16 @@
       <c r="K97" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L97" s="189">
+      <c r="L97" s="108">
         <v>2014.2804877190592</v>
       </c>
-      <c r="M97" s="189">
+      <c r="M97" s="108">
         <v>2014.2804877190592</v>
       </c>
-      <c r="N97" s="189">
+      <c r="N97" s="108">
         <v>2014.2804877190592</v>
       </c>
-      <c r="O97" s="189">
+      <c r="O97" s="108">
         <v>2014.2804877190592</v>
       </c>
       <c r="P97" t="str">
@@ -45199,16 +45380,16 @@
       <c r="K98" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L98" s="190">
+      <c r="L98" s="109">
         <v>1.5565575501406395</v>
       </c>
-      <c r="M98" s="190">
+      <c r="M98" s="109">
         <v>1.2510982334688685</v>
       </c>
-      <c r="N98" s="190">
+      <c r="N98" s="109">
         <v>1.1609021481572299</v>
       </c>
-      <c r="O98" s="190">
+      <c r="O98" s="109">
         <v>1.0898970686435683</v>
       </c>
       <c r="P98" t="str">
@@ -45243,16 +45424,16 @@
       <c r="K99" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L99" s="192">
+      <c r="L99" s="107">
         <v>194.09413912347242</v>
       </c>
-      <c r="M99" s="192">
+      <c r="M99" s="107">
         <v>194.09413912347242</v>
       </c>
-      <c r="N99" s="192">
+      <c r="N99" s="107">
         <v>194.09413912347242</v>
       </c>
-      <c r="O99" s="192">
+      <c r="O99" s="107">
         <v>194.09413912347242</v>
       </c>
       <c r="P99" t="str">
@@ -45293,16 +45474,16 @@
       <c r="K100" s="103" t="s">
         <v>133</v>
       </c>
-      <c r="L100" s="192">
+      <c r="L100" s="107">
         <v>16645.181656612192</v>
       </c>
-      <c r="M100" s="192">
+      <c r="M100" s="107">
         <v>16645.181656612192</v>
       </c>
-      <c r="N100" s="192">
+      <c r="N100" s="107">
         <v>16645.181656612192</v>
       </c>
-      <c r="O100" s="192">
+      <c r="O100" s="107">
         <v>16645.181656612192</v>
       </c>
       <c r="P100" t="str">
@@ -45327,10 +45508,10 @@
       <c r="I101" s="106"/>
       <c r="J101" s="103"/>
       <c r="K101" s="103"/>
-      <c r="L101" s="195"/>
-      <c r="M101" s="195"/>
-      <c r="N101" s="195"/>
-      <c r="O101" s="195"/>
+      <c r="L101" s="111"/>
+      <c r="M101" s="111"/>
+      <c r="N101" s="111"/>
+      <c r="O101" s="111"/>
       <c r="U101" s="144">
         <v>23505.4</v>
       </c>
@@ -45365,16 +45546,16 @@
       <c r="K102" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L102" s="190">
+      <c r="L102" s="109">
         <v>0.62347491540903066</v>
       </c>
-      <c r="M102" s="190">
+      <c r="M102" s="109">
         <v>0.62347491540903066</v>
       </c>
-      <c r="N102" s="190">
+      <c r="N102" s="109">
         <v>0.62347491540903066</v>
       </c>
-      <c r="O102" s="190">
+      <c r="O102" s="109">
         <v>0.62347491540903066</v>
       </c>
       <c r="P102" t="str">
@@ -45419,16 +45600,16 @@
       <c r="K103" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L103" s="190">
+      <c r="L103" s="109">
         <v>0.62347491540903066</v>
       </c>
-      <c r="M103" s="190">
+      <c r="M103" s="109">
         <v>0.62347491540903066</v>
       </c>
-      <c r="N103" s="190">
+      <c r="N103" s="109">
         <v>0.62347491540903066</v>
       </c>
-      <c r="O103" s="190">
+      <c r="O103" s="109">
         <v>0.62347491540903066</v>
       </c>
       <c r="P103" t="str">
@@ -45467,16 +45648,16 @@
       <c r="K104" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L104" s="188">
+      <c r="L104" s="110">
         <v>14795</v>
       </c>
-      <c r="M104" s="188">
+      <c r="M104" s="110">
         <v>14795</v>
       </c>
-      <c r="N104" s="188">
+      <c r="N104" s="110">
         <v>14795</v>
       </c>
-      <c r="O104" s="188">
+      <c r="O104" s="110">
         <v>14795</v>
       </c>
       <c r="P104" t="str">
@@ -45521,16 +45702,16 @@
       <c r="K105" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L105" s="192">
+      <c r="L105" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="M105" s="192">
+      <c r="M105" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="N105" s="192">
+      <c r="N105" s="107">
         <v>-123.29166666666667</v>
       </c>
-      <c r="O105" s="192">
+      <c r="O105" s="107">
         <v>-123.29166666666667</v>
       </c>
       <c r="P105" t="str">
@@ -45559,10 +45740,10 @@
         <v>4</v>
       </c>
       <c r="K106" s="103"/>
-      <c r="L106" s="191"/>
-      <c r="M106" s="191"/>
-      <c r="N106" s="191"/>
-      <c r="O106" s="191"/>
+      <c r="L106" s="104"/>
+      <c r="M106" s="104"/>
+      <c r="N106" s="104"/>
+      <c r="O106" s="104"/>
       <c r="P106" t="str">
         <f t="shared" si="5"/>
         <v/>
@@ -45601,16 +45782,16 @@
       <c r="K107" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L107" s="192">
+      <c r="L107" s="107">
         <v>-910.87097763578595</v>
       </c>
-      <c r="M107" s="192">
+      <c r="M107" s="107">
         <v>-785.99515987377549</v>
       </c>
-      <c r="N107" s="192">
+      <c r="N107" s="107">
         <v>-812.7200382800246</v>
       </c>
-      <c r="O107" s="192">
+      <c r="O107" s="107">
         <v>-697.66182895837528</v>
       </c>
       <c r="P107" t="str">
@@ -45651,16 +45832,16 @@
       <c r="K108" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L108" s="190">
+      <c r="L108" s="109">
         <v>3.7835923922104817E-2</v>
       </c>
-      <c r="M108" s="190">
+      <c r="M108" s="109">
         <v>1.6649895128467544E-2</v>
       </c>
-      <c r="N108" s="190">
+      <c r="N108" s="109">
         <v>1.0726800574048566E-2</v>
       </c>
-      <c r="O108" s="190">
+      <c r="O108" s="109">
         <v>1.6954573220574328E-3</v>
       </c>
       <c r="P108" t="str">
@@ -45701,16 +45882,16 @@
       <c r="K109" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L109" s="189">
+      <c r="L109" s="108">
         <v>2785.1006045537742</v>
       </c>
-      <c r="M109" s="189">
+      <c r="M109" s="108">
         <v>2794.4830281684162</v>
       </c>
-      <c r="N109" s="189">
+      <c r="N109" s="108">
         <v>2796.3023196738063</v>
       </c>
-      <c r="O109" s="189">
+      <c r="O109" s="108">
         <v>2799.5130899513856</v>
       </c>
       <c r="P109" t="str">
@@ -45754,16 +45935,16 @@
       <c r="K110" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L110" s="200">
+      <c r="L110" s="113">
         <v>8.0055136256249507E-2</v>
       </c>
-      <c r="M110" s="200">
+      <c r="M110" s="113">
         <v>6.736187417227342E-2</v>
       </c>
-      <c r="N110" s="200">
+      <c r="N110" s="113">
         <v>7.0078379992635012E-2</v>
       </c>
-      <c r="O110" s="200">
+      <c r="O110" s="113">
         <v>5.8383049127086306E-2</v>
       </c>
       <c r="P110" t="str">
@@ -45808,16 +45989,16 @@
       <c r="K111" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L111" s="200">
+      <c r="L111" s="113">
         <v>8.0055136256249507E-2</v>
       </c>
-      <c r="M111" s="200">
+      <c r="M111" s="113">
         <v>6.736187417227342E-2</v>
       </c>
-      <c r="N111" s="200">
+      <c r="N111" s="113">
         <v>7.0078379992635012E-2</v>
       </c>
-      <c r="O111" s="200">
+      <c r="O111" s="113">
         <v>5.8383049127086306E-2</v>
       </c>
       <c r="P111" t="str">
@@ -45859,10 +46040,10 @@
       <c r="K112" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L112" s="196"/>
-      <c r="M112" s="196"/>
-      <c r="N112" s="196"/>
-      <c r="O112" s="196"/>
+      <c r="L112" s="128"/>
+      <c r="M112" s="128"/>
+      <c r="N112" s="128"/>
+      <c r="O112" s="128"/>
       <c r="P112" t="str">
         <f t="shared" si="5"/>
         <v>Bending moment L-Flange as a function of external force Z</v>
@@ -45901,16 +46082,16 @@
       <c r="K113" s="103" t="s">
         <v>125</v>
       </c>
-      <c r="L113" s="192">
+      <c r="L113" s="107">
         <v>90.212333179266878</v>
       </c>
-      <c r="M113" s="192">
+      <c r="M113" s="107">
         <v>90.212333179266878</v>
       </c>
-      <c r="N113" s="192">
+      <c r="N113" s="107">
         <v>90.212333179266878</v>
       </c>
-      <c r="O113" s="192">
+      <c r="O113" s="107">
         <v>90.212333179266878</v>
       </c>
       <c r="P113" t="str">
@@ -45948,16 +46129,16 @@
       <c r="K114" s="103" t="s">
         <v>267</v>
       </c>
-      <c r="L114" s="194">
+      <c r="L114" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="M114" s="194">
+      <c r="M114" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="N114" s="194">
+      <c r="N114" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
-      <c r="O114" s="194">
+      <c r="O114" s="114">
         <v>1.6641565715404047E-9</v>
       </c>
       <c r="P114" t="str">
@@ -45999,10 +46180,10 @@
       <c r="K115" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L115" s="196"/>
-      <c r="M115" s="196"/>
-      <c r="N115" s="196"/>
-      <c r="O115" s="196"/>
+      <c r="L115" s="128"/>
+      <c r="M115" s="128"/>
+      <c r="N115" s="128"/>
+      <c r="O115" s="128"/>
       <c r="P115" t="str">
         <f t="shared" si="5"/>
         <v>Bending moment for T-Flange as a function of external force Z</v>
@@ -46042,10 +46223,10 @@
       <c r="K116" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L116" s="196"/>
-      <c r="M116" s="196"/>
-      <c r="N116" s="196"/>
-      <c r="O116" s="196"/>
+      <c r="L116" s="128"/>
+      <c r="M116" s="128"/>
+      <c r="N116" s="128"/>
+      <c r="O116" s="128"/>
       <c r="P116" t="str">
         <f t="shared" si="5"/>
         <v>Intermediate values as function of Z</v>
@@ -46085,10 +46266,10 @@
       <c r="K117" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L117" s="196"/>
-      <c r="M117" s="196"/>
-      <c r="N117" s="196"/>
-      <c r="O117" s="196"/>
+      <c r="L117" s="128"/>
+      <c r="M117" s="128"/>
+      <c r="N117" s="128"/>
+      <c r="O117" s="128"/>
       <c r="P117" t="str">
         <f t="shared" si="5"/>
         <v>Intermediate values as function of Z</v>
@@ -46130,16 +46311,16 @@
       <c r="K118" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L118" s="190">
+      <c r="L118" s="109">
         <v>0.2894651978787075</v>
       </c>
-      <c r="M118" s="190">
+      <c r="M118" s="109">
         <v>0.24167020477805987</v>
       </c>
-      <c r="N118" s="190">
+      <c r="N118" s="109">
         <v>0.23234521741945613</v>
       </c>
-      <c r="O118" s="190">
+      <c r="O118" s="109">
         <v>0.20959328922292766</v>
       </c>
       <c r="P118" t="str">
@@ -46175,16 +46356,16 @@
       <c r="K119" s="103" t="s">
         <v>122</v>
       </c>
-      <c r="L119" s="194">
+      <c r="L119" s="114">
         <v>0.1764573607132747</v>
       </c>
-      <c r="M119" s="194">
+      <c r="M119" s="114">
         <v>0.14750866143207148</v>
       </c>
-      <c r="N119" s="194">
+      <c r="N119" s="114">
         <v>0.15173499245887154</v>
       </c>
-      <c r="O119" s="194">
+      <c r="O119" s="114">
         <v>0.12314892797409971</v>
       </c>
       <c r="P119" t="str">
@@ -46228,16 +46409,16 @@
       <c r="K120" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L120" s="189">
+      <c r="L120" s="108">
         <v>-131.51232454134481</v>
       </c>
-      <c r="M120" s="189">
+      <c r="M120" s="108">
         <v>-101.8802860790333</v>
       </c>
-      <c r="N120" s="189">
+      <c r="N120" s="108">
         <v>-103.58907088530368</v>
       </c>
-      <c r="O120" s="189">
+      <c r="O120" s="108">
         <v>-85.219196302762441</v>
       </c>
       <c r="P120" t="str">
@@ -46273,16 +46454,16 @@
       <c r="K121" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L121" s="189">
+      <c r="L121" s="108">
         <v>-90.981881194694239</v>
       </c>
-      <c r="M121" s="189">
+      <c r="M121" s="108">
         <v>-69.170797745127899</v>
       </c>
-      <c r="N121" s="189">
+      <c r="N121" s="108">
         <v>-73.788867024160552</v>
       </c>
-      <c r="O121" s="189">
+      <c r="O121" s="108">
         <v>-54.472533054425661</v>
       </c>
       <c r="P121" t="str">
@@ -46315,16 +46496,16 @@
       <c r="K122" s="103" t="s">
         <v>127</v>
       </c>
-      <c r="L122" s="190">
+      <c r="L122" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="M122" s="190">
+      <c r="M122" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="N122" s="190">
+      <c r="N122" s="109">
         <v>-123.19166666666668</v>
       </c>
-      <c r="O122" s="190">
+      <c r="O122" s="109">
         <v>-123.19166666666668</v>
       </c>
       <c r="U122" s="144">
@@ -46356,16 +46537,16 @@
       <c r="K123" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L123" s="200">
-        <v>0</v>
-      </c>
-      <c r="M123" s="200">
-        <v>0</v>
-      </c>
-      <c r="N123" s="200">
-        <v>0</v>
-      </c>
-      <c r="O123" s="200">
+      <c r="L123" s="113">
+        <v>0</v>
+      </c>
+      <c r="M123" s="113">
+        <v>0</v>
+      </c>
+      <c r="N123" s="113">
+        <v>0</v>
+      </c>
+      <c r="O123" s="113">
         <v>0</v>
       </c>
       <c r="P123" s="142" t="s">
@@ -46400,16 +46581,16 @@
       <c r="K124" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L124" s="190">
+      <c r="L124" s="109">
         <v>-79.8339147984276</v>
       </c>
-      <c r="M124" s="190">
+      <c r="M124" s="109">
         <v>-85.75104981737654</v>
       </c>
-      <c r="N124" s="190">
+      <c r="N124" s="109">
         <v>-88.093742708092066</v>
       </c>
-      <c r="O124" s="190">
+      <c r="O124" s="109">
         <v>-90.210753224210066</v>
       </c>
       <c r="P124" s="142" t="s">
@@ -46444,16 +46625,16 @@
       <c r="K125" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L125" s="200">
+      <c r="L125" s="113">
         <v>-21.494797911699134</v>
       </c>
-      <c r="M125" s="200">
+      <c r="M125" s="113">
         <v>-20.293545140458644</v>
       </c>
-      <c r="N125" s="200">
+      <c r="N125" s="113">
         <v>-21.483662640318066</v>
       </c>
-      <c r="O125" s="200">
+      <c r="O125" s="113">
         <v>-19.105998181158864</v>
       </c>
       <c r="P125" s="142" t="s">
@@ -46488,16 +46669,16 @@
       <c r="K126" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L126" s="200">
+      <c r="L126" s="113">
         <v>4.0215592424512944E-3</v>
       </c>
-      <c r="M126" s="200">
+      <c r="M126" s="113">
         <v>1.7697080630985826E-3</v>
       </c>
-      <c r="N126" s="200">
+      <c r="N126" s="113">
         <v>1.1401456478057396E-3</v>
       </c>
-      <c r="O126" s="200">
+      <c r="O126" s="113">
         <v>1.8020921275080322E-4</v>
       </c>
       <c r="P126" s="142" t="s">
@@ -46532,16 +46713,16 @@
       <c r="K127" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L127" s="190">
+      <c r="L127" s="109">
         <v>-79.769162721538052</v>
       </c>
-      <c r="M127" s="190">
+      <c r="M127" s="109">
         <v>-85.681498442059961</v>
       </c>
-      <c r="N127" s="190">
+      <c r="N127" s="109">
         <v>-88.02229121011996</v>
       </c>
-      <c r="O127" s="190">
+      <c r="O127" s="109">
         <v>-90.137584651131959</v>
       </c>
       <c r="P127" s="142" t="s">
@@ -46576,16 +46757,16 @@
       <c r="K128" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L128" s="200">
+      <c r="L128" s="113">
         <v>-21.477152175627808</v>
       </c>
-      <c r="M128" s="200">
+      <c r="M128" s="113">
         <v>-20.278794274315437</v>
       </c>
-      <c r="N128" s="200">
+      <c r="N128" s="113">
         <v>-21.46848914107218</v>
       </c>
-      <c r="O128" s="200">
+      <c r="O128" s="113">
         <v>-19.093683288361454</v>
       </c>
       <c r="P128" s="142" t="s">
@@ -46617,16 +46798,16 @@
       <c r="K129" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L129" s="189">
+      <c r="L129" s="108">
         <v>-17.523923993918729</v>
       </c>
-      <c r="M129" s="189">
+      <c r="M129" s="108">
         <v>-21.802441623784492</v>
       </c>
-      <c r="N129" s="189">
+      <c r="N129" s="108">
         <v>-23.49637843648005</v>
       </c>
-      <c r="O129" s="189">
+      <c r="O129" s="108">
         <v>-25.027130529649465</v>
       </c>
       <c r="U129" s="144">
@@ -46655,16 +46836,16 @@
       <c r="K130" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L130" s="189">
+      <c r="L130" s="108">
         <v>2997.1619494237261</v>
       </c>
-      <c r="M130" s="189">
+      <c r="M130" s="108">
         <v>3024.7894225430455</v>
       </c>
-      <c r="N130" s="189">
+      <c r="N130" s="108">
         <v>3018.8768217447646</v>
       </c>
-      <c r="O130" s="189">
+      <c r="O130" s="108">
         <v>3044.3322513240018</v>
       </c>
       <c r="U130" s="144">
@@ -46693,16 +46874,16 @@
       <c r="K131" s="103" t="s">
         <v>120</v>
       </c>
-      <c r="L131" s="189">
+      <c r="L131" s="108">
         <v>109.5849335870903</v>
       </c>
-      <c r="M131" s="189">
+      <c r="M131" s="108">
         <v>87.672945630325998</v>
       </c>
-      <c r="N131" s="189">
+      <c r="N131" s="108">
         <v>87.831110336558268</v>
       </c>
-      <c r="O131" s="189">
+      <c r="O131" s="108">
         <v>75.265892523267908</v>
       </c>
       <c r="U131" s="144">
@@ -46728,16 +46909,16 @@
       <c r="J132" s="112" t="s">
         <v>344</v>
       </c>
-      <c r="L132" s="199">
+      <c r="L132" s="135">
         <v>5.8722784924298643E-4</v>
       </c>
-      <c r="M132" s="199">
+      <c r="M132" s="135">
         <v>7.9243250356270795E-4</v>
       </c>
-      <c r="N132" s="199">
+      <c r="N132" s="135">
         <v>9.6252341234037329E-4</v>
       </c>
-      <c r="O132" s="199">
+      <c r="O132" s="135">
         <v>9.4754125098918721E-4</v>
       </c>
       <c r="P132" t="s">
@@ -46766,16 +46947,16 @@
       <c r="J133" s="112" t="s">
         <v>343</v>
       </c>
-      <c r="L133" s="199">
+      <c r="L133" s="135">
         <v>0.43420707559348615</v>
       </c>
-      <c r="M133" s="199">
+      <c r="M133" s="135">
         <v>0.43699160968249873</v>
       </c>
-      <c r="N133" s="199">
+      <c r="N133" s="135">
         <v>0.46959119650800563</v>
       </c>
-      <c r="O133" s="199">
+      <c r="O133" s="135">
         <v>0.44314641525918591</v>
       </c>
       <c r="P133" t="s">
@@ -46804,16 +46985,16 @@
       <c r="J134" s="112" t="s">
         <v>342</v>
       </c>
-      <c r="L134" s="199">
+      <c r="L134" s="135">
         <v>27.0838363499347</v>
       </c>
-      <c r="M134" s="199">
+      <c r="M134" s="135">
         <v>20.029346462996614</v>
       </c>
-      <c r="N134" s="199">
+      <c r="N134" s="135">
         <v>19.769143191521266</v>
       </c>
-      <c r="O134" s="199">
+      <c r="O134" s="135">
         <v>15.20571130723215</v>
       </c>
       <c r="P134" t="s">
@@ -46832,10 +47013,10 @@
     <row r="135" spans="3:23">
       <c r="C135" s="112"/>
       <c r="J135" s="112"/>
-      <c r="L135" s="197"/>
-      <c r="M135" s="197"/>
-      <c r="N135" s="197"/>
-      <c r="O135" s="197"/>
+      <c r="L135" s="112"/>
+      <c r="M135" s="112"/>
+      <c r="N135" s="112"/>
+      <c r="O135" s="112"/>
       <c r="U135" s="144">
         <v>2.1692199999999998E-2</v>
       </c>
@@ -46861,16 +47042,16 @@
         <v>92</v>
       </c>
       <c r="K136" s="164"/>
-      <c r="L136" s="190">
+      <c r="L136" s="109">
         <v>1.4812583073587486</v>
       </c>
-      <c r="M136" s="190">
+      <c r="M136" s="109">
         <v>3.2501218122193491</v>
       </c>
-      <c r="N136" s="190">
+      <c r="N136" s="109">
         <v>6.014862663421173</v>
       </c>
-      <c r="O136" s="190">
+      <c r="O136" s="109">
         <v>5.286104670707072</v>
       </c>
       <c r="P136" t="s">
@@ -58860,6 +59041,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101004E5A98ECA1EC044BB77E0D7F6ADEF7BC" ma:contentTypeVersion="18" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="5e88349ac6f5efd4674595e2a92e1fa9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2278e7f3-5df8-4100-b836-5320443b7544" xmlns:ns4="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bde21b231255bb48ab8a6ec7dd561648" ns3:_="" ns4:_="">
     <xsd:import namespace="2278e7f3-5df8-4100-b836-5320443b7544"/>
@@ -59112,14 +59301,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="2278e7f3-5df8-4100-b836-5320443b7544" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52E10DE4-EB42-4EC5-8AEE-EE77FE7979AC}">
   <ds:schemaRefs>
@@ -59129,6 +59310,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
+    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A7863D2-B6F1-4C67-B9E9-1F3A9276C4FF}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -59145,21 +59343,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D3A318F-BD98-4749-9B6A-DFC991AC8E75}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3fb9cbd1-4a98-4945-a235-2d8a3d5ec2be"/>
-    <ds:schemaRef ds:uri="2278e7f3-5df8-4100-b836-5320443b7544"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>